<commit_message>
Ben added to dictionary
</commit_message>
<xml_diff>
--- a/Outputs/stacks_over_time_avg.xlsx
+++ b/Outputs/stacks_over_time_avg.xlsx
@@ -194,7 +194,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$B$2:$B$156</f>
+              <f>'data'!$B$2:$B$189</f>
             </numRef>
           </val>
         </ser>
@@ -221,7 +221,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$C$2:$C$156</f>
+              <f>'data'!$C$2:$C$189</f>
             </numRef>
           </val>
         </ser>
@@ -248,7 +248,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$D$2:$D$156</f>
+              <f>'data'!$D$2:$D$189</f>
             </numRef>
           </val>
         </ser>
@@ -275,7 +275,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$E$2:$E$156</f>
+              <f>'data'!$E$2:$E$189</f>
             </numRef>
           </val>
         </ser>
@@ -302,61 +302,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$F$2:$F$156</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <strRef>
-              <f>'data'!G1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'data'!$G$2:$G$156</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="6"/>
-          <order val="6"/>
-          <tx>
-            <strRef>
-              <f>'data'!H1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'data'!$H$2:$H$156</f>
+              <f>'data'!$F$2:$F$189</f>
             </numRef>
           </val>
         </ser>
@@ -726,7 +672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H156"/>
+  <dimension ref="A1:F189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -742,37 +688,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Raymond</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Regan</t>
+          <t>Ben</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fish</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Cedric</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Fish</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Cheyenne</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Scott</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Jacob</t>
+          <t>Raymond</t>
         </is>
       </c>
     </row>
@@ -798,16 +734,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="D3" t="n">
         <v>20</v>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
         <v>20</v>
-      </c>
-      <c r="D3" t="n">
-        <v>19.95</v>
-      </c>
-      <c r="E3" t="n">
-        <v>20.05</v>
       </c>
     </row>
     <row r="4">
@@ -815,16 +751,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20.78</v>
+        <v>20.67</v>
       </c>
       <c r="C4" t="n">
-        <v>19.93</v>
+        <v>19.33</v>
       </c>
       <c r="D4" t="n">
-        <v>19.93</v>
+        <v>20</v>
       </c>
       <c r="E4" t="n">
-        <v>19.35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -832,16 +768,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>21.15</v>
+        <v>21.2</v>
       </c>
       <c r="C5" t="n">
-        <v>19.98</v>
+        <v>19.05</v>
       </c>
       <c r="D5" t="n">
-        <v>19.92</v>
+        <v>19.8</v>
       </c>
       <c r="E5" t="n">
-        <v>18.95</v>
+        <v>19.95</v>
       </c>
     </row>
     <row r="6">
@@ -849,16 +785,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>21.37</v>
+        <v>21.44</v>
       </c>
       <c r="C6" t="n">
-        <v>19.96</v>
+        <v>18.84</v>
       </c>
       <c r="D6" t="n">
-        <v>19.96</v>
+        <v>19.68</v>
       </c>
       <c r="E6" t="n">
-        <v>18.71</v>
+        <v>20.04</v>
       </c>
     </row>
     <row r="7">
@@ -866,16 +802,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>21.52</v>
+        <v>21.15</v>
       </c>
       <c r="C7" t="n">
-        <v>19.95</v>
+        <v>17.92</v>
       </c>
       <c r="D7" t="n">
-        <v>19.95</v>
+        <v>20.83</v>
       </c>
       <c r="E7" t="n">
-        <v>18.58</v>
+        <v>20.1</v>
       </c>
     </row>
     <row r="8">
@@ -883,16 +819,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>21.59</v>
+        <v>20.94</v>
       </c>
       <c r="C8" t="n">
-        <v>19.94</v>
+        <v>17.2</v>
       </c>
       <c r="D8" t="n">
-        <v>19.94</v>
+        <v>21.71</v>
       </c>
       <c r="E8" t="n">
-        <v>18.52</v>
+        <v>20.14</v>
       </c>
     </row>
     <row r="9">
@@ -900,16 +836,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>21.64</v>
+        <v>21.01</v>
       </c>
       <c r="C9" t="n">
-        <v>20.09</v>
+        <v>16.56</v>
       </c>
       <c r="D9" t="n">
-        <v>19.94</v>
+        <v>22.28</v>
       </c>
       <c r="E9" t="n">
-        <v>18.33</v>
+        <v>20.15</v>
       </c>
     </row>
     <row r="10">
@@ -917,16 +853,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>21.67</v>
+        <v>20.88</v>
       </c>
       <c r="C10" t="n">
-        <v>20.19</v>
+        <v>16.29</v>
       </c>
       <c r="D10" t="n">
-        <v>19.98</v>
+        <v>22.69</v>
       </c>
       <c r="E10" t="n">
-        <v>18.16</v>
+        <v>20.14</v>
       </c>
     </row>
     <row r="11">
@@ -934,16 +870,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>21.73</v>
+        <v>21.06</v>
       </c>
       <c r="C11" t="n">
-        <v>20.27</v>
+        <v>16.05</v>
       </c>
       <c r="D11" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E11" t="n">
-        <v>18.01</v>
+        <v>19.89</v>
       </c>
     </row>
     <row r="12">
@@ -951,16 +887,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>21.73</v>
+        <v>21.06</v>
       </c>
       <c r="C12" t="n">
-        <v>20.27</v>
+        <v>16.05</v>
       </c>
       <c r="D12" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E12" t="n">
-        <v>18.01</v>
+        <v>19.89</v>
       </c>
     </row>
     <row r="13">
@@ -968,16 +904,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>21.93</v>
+        <v>21.32</v>
       </c>
       <c r="C13" t="n">
-        <v>20.36</v>
+        <v>15.47</v>
       </c>
       <c r="D13" t="n">
-        <v>20.02</v>
+        <v>23.56</v>
       </c>
       <c r="E13" t="n">
-        <v>17.68</v>
+        <v>19.65</v>
       </c>
     </row>
     <row r="14">
@@ -985,16 +921,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>22.13</v>
+        <v>21.23</v>
       </c>
       <c r="C14" t="n">
-        <v>20.38</v>
+        <v>14.92</v>
       </c>
       <c r="D14" t="n">
-        <v>20.05</v>
+        <v>24.46</v>
       </c>
       <c r="E14" t="n">
-        <v>17.45</v>
+        <v>19.39</v>
       </c>
     </row>
     <row r="15">
@@ -1002,16 +938,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>22.09</v>
+        <v>21.2</v>
       </c>
       <c r="C15" t="n">
-        <v>20.51</v>
+        <v>14.37</v>
       </c>
       <c r="D15" t="n">
-        <v>20.03</v>
+        <v>25.31</v>
       </c>
       <c r="E15" t="n">
-        <v>17.37</v>
+        <v>19.12</v>
       </c>
     </row>
     <row r="16">
@@ -1019,16 +955,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>22.06</v>
+        <v>21.14</v>
       </c>
       <c r="C16" t="n">
-        <v>20.69</v>
+        <v>13.88</v>
       </c>
       <c r="D16" t="n">
-        <v>19.99</v>
+        <v>26.11</v>
       </c>
       <c r="E16" t="n">
-        <v>17.26</v>
+        <v>18.87</v>
       </c>
     </row>
     <row r="17">
@@ -1036,16 +972,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>22.01</v>
+        <v>21.12</v>
       </c>
       <c r="C17" t="n">
-        <v>20.89</v>
+        <v>13.43</v>
       </c>
       <c r="D17" t="n">
-        <v>19.97</v>
+        <v>26.91</v>
       </c>
       <c r="E17" t="n">
-        <v>17.13</v>
+        <v>18.56</v>
       </c>
     </row>
     <row r="18">
@@ -1053,16 +989,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>21.95</v>
+        <v>22.27</v>
       </c>
       <c r="C18" t="n">
-        <v>21.05</v>
+        <v>12.58</v>
       </c>
       <c r="D18" t="n">
-        <v>20.02</v>
+        <v>26.96</v>
       </c>
       <c r="E18" t="n">
-        <v>16.98</v>
+        <v>18.23</v>
       </c>
     </row>
     <row r="19">
@@ -1070,16 +1006,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>21.84</v>
+        <v>23.37</v>
       </c>
       <c r="C19" t="n">
-        <v>21.2</v>
+        <v>11.7</v>
       </c>
       <c r="D19" t="n">
-        <v>20</v>
+        <v>26.96</v>
       </c>
       <c r="E19" t="n">
-        <v>16.96</v>
+        <v>18.02</v>
       </c>
     </row>
     <row r="20">
@@ -1087,16 +1023,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>21.77</v>
+        <v>24.43</v>
       </c>
       <c r="C20" t="n">
-        <v>21.22</v>
+        <v>10.78</v>
       </c>
       <c r="D20" t="n">
-        <v>19.97</v>
+        <v>27</v>
       </c>
       <c r="E20" t="n">
-        <v>17.04</v>
+        <v>17.83</v>
       </c>
     </row>
     <row r="21">
@@ -1104,16 +1040,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>21.91</v>
+        <v>26.44</v>
       </c>
       <c r="C21" t="n">
-        <v>21.25</v>
+        <v>9.65</v>
       </c>
       <c r="D21" t="n">
-        <v>19.79</v>
+        <v>26.3</v>
       </c>
       <c r="E21" t="n">
-        <v>17.04</v>
+        <v>17.65</v>
       </c>
     </row>
     <row r="22">
@@ -1121,16 +1057,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>21.91</v>
+        <v>28.16</v>
       </c>
       <c r="C22" t="n">
-        <v>21.4</v>
+        <v>8.52</v>
       </c>
       <c r="D22" t="n">
-        <v>19.63</v>
+        <v>25.61</v>
       </c>
       <c r="E22" t="n">
-        <v>17.06</v>
+        <v>17.76</v>
       </c>
     </row>
     <row r="23">
@@ -1138,16 +1074,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>21.92</v>
+        <v>29.61</v>
       </c>
       <c r="C23" t="n">
-        <v>21.53</v>
+        <v>7.71</v>
       </c>
       <c r="D23" t="n">
-        <v>19.51</v>
+        <v>24.87</v>
       </c>
       <c r="E23" t="n">
-        <v>17.04</v>
+        <v>17.86</v>
       </c>
     </row>
     <row r="24">
@@ -1155,16 +1091,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>21.94</v>
+        <v>32.01</v>
       </c>
       <c r="C24" t="n">
-        <v>21.74</v>
+        <v>6.35</v>
       </c>
       <c r="D24" t="n">
-        <v>19.31</v>
+        <v>23.7</v>
       </c>
       <c r="E24" t="n">
-        <v>17.01</v>
+        <v>17.98</v>
       </c>
     </row>
     <row r="25">
@@ -1172,16 +1108,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>21.92</v>
+        <v>34.37</v>
       </c>
       <c r="C25" t="n">
-        <v>21.85</v>
+        <v>5</v>
       </c>
       <c r="D25" t="n">
-        <v>19.23</v>
+        <v>22.56</v>
       </c>
       <c r="E25" t="n">
-        <v>17.01</v>
+        <v>18.11</v>
       </c>
     </row>
     <row r="26">
@@ -1189,19 +1125,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>21.88</v>
+        <v>36.6</v>
       </c>
       <c r="C26" t="n">
-        <v>22.32</v>
+        <v>3.67</v>
       </c>
       <c r="D26" t="n">
-        <v>18.76</v>
+        <v>21.55</v>
       </c>
       <c r="E26" t="n">
-        <v>17.04</v>
-      </c>
-      <c r="F26" t="n">
-        <v>20</v>
+        <v>18.22</v>
       </c>
     </row>
     <row r="27">
@@ -1209,19 +1142,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>21.84</v>
+        <v>38.81</v>
       </c>
       <c r="C27" t="n">
-        <v>22.45</v>
+        <v>2.32</v>
       </c>
       <c r="D27" t="n">
-        <v>18.68</v>
+        <v>20.57</v>
       </c>
       <c r="E27" t="n">
-        <v>17.04</v>
-      </c>
-      <c r="F27" t="n">
-        <v>19.9</v>
+        <v>18.32</v>
       </c>
     </row>
     <row r="28">
@@ -1229,19 +1159,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>21.82</v>
+        <v>39.82</v>
       </c>
       <c r="C28" t="n">
-        <v>22.61</v>
+        <v>1.85</v>
       </c>
       <c r="D28" t="n">
-        <v>18.53</v>
+        <v>19.89</v>
       </c>
       <c r="E28" t="n">
-        <v>17.06</v>
-      </c>
-      <c r="F28" t="n">
-        <v>19.53333333333333</v>
+        <v>18.44</v>
       </c>
     </row>
     <row r="29">
@@ -1249,19 +1176,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>21.84</v>
+        <v>40.9</v>
       </c>
       <c r="C29" t="n">
-        <v>21.4</v>
+        <v>1.44</v>
       </c>
       <c r="D29" t="n">
-        <v>18.46</v>
+        <v>19.22</v>
       </c>
       <c r="E29" t="n">
-        <v>18.43</v>
-      </c>
-      <c r="F29" t="n">
-        <v>19.525</v>
+        <v>18.45</v>
       </c>
     </row>
     <row r="30">
@@ -1269,19 +1193,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>21.83</v>
+        <v>41.83</v>
       </c>
       <c r="C30" t="n">
-        <v>20.16</v>
+        <v>1.14</v>
       </c>
       <c r="D30" t="n">
-        <v>18.4</v>
+        <v>18.58</v>
       </c>
       <c r="E30" t="n">
-        <v>19.8</v>
-      </c>
-      <c r="F30" t="n">
-        <v>19.44</v>
+        <v>18.45</v>
       </c>
     </row>
     <row r="31">
@@ -1289,19 +1210,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>21.59</v>
+        <v>42.03</v>
       </c>
       <c r="C31" t="n">
-        <v>19.01</v>
+        <v>0.86</v>
       </c>
       <c r="D31" t="n">
+        <v>18.68</v>
+      </c>
+      <c r="E31" t="n">
         <v>18.43</v>
-      </c>
-      <c r="E31" t="n">
-        <v>21.25</v>
-      </c>
-      <c r="F31" t="n">
-        <v>19.38333333333333</v>
       </c>
     </row>
     <row r="32">
@@ -1309,19 +1227,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>21.64</v>
+        <v>42.23</v>
       </c>
       <c r="C32" t="n">
-        <v>17.73</v>
+        <v>0.6</v>
       </c>
       <c r="D32" t="n">
-        <v>18.43</v>
+        <v>18.48</v>
       </c>
       <c r="E32" t="n">
-        <v>22.57</v>
-      </c>
-      <c r="F32" t="n">
-        <v>19.34285714285715</v>
+        <v>18.69</v>
       </c>
     </row>
     <row r="33">
@@ -1329,19 +1244,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>21.65</v>
+        <v>42.05</v>
       </c>
       <c r="C33" t="n">
-        <v>16.52</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
         <v>18.35</v>
       </c>
       <c r="E33" t="n">
-        <v>23.95</v>
-      </c>
-      <c r="F33" t="n">
-        <v>19.2875</v>
+        <v>19.6</v>
       </c>
     </row>
     <row r="34">
@@ -1349,19 +1261,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>21.59</v>
+        <v>41.21</v>
       </c>
       <c r="C34" t="n">
-        <v>15.21</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>18.35</v>
+        <v>18.28</v>
       </c>
       <c r="E34" t="n">
-        <v>25.42</v>
-      </c>
-      <c r="F34" t="n">
-        <v>19.45555555555556</v>
+        <v>20.51</v>
       </c>
     </row>
     <row r="35">
@@ -1369,19 +1278,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>21.55</v>
+        <v>40.35</v>
       </c>
       <c r="C35" t="n">
-        <v>13.74</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>18.28</v>
+        <v>18.21</v>
       </c>
       <c r="E35" t="n">
-        <v>26.92</v>
-      </c>
-      <c r="F35" t="n">
-        <v>19.58</v>
+        <v>21.44</v>
       </c>
     </row>
     <row r="36">
@@ -1389,19 +1295,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>21.52</v>
+        <v>39.47</v>
       </c>
       <c r="C36" t="n">
-        <v>11.89</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>18.61</v>
+        <v>18.15</v>
       </c>
       <c r="E36" t="n">
-        <v>28.39</v>
-      </c>
-      <c r="F36" t="n">
-        <v>19.58</v>
+        <v>22.38</v>
       </c>
     </row>
     <row r="37">
@@ -1409,22 +1312,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>21.54</v>
+        <v>38.69</v>
       </c>
       <c r="C37" t="n">
-        <v>10.38</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>18.5</v>
+        <v>17.98</v>
       </c>
       <c r="E37" t="n">
-        <v>29.93</v>
-      </c>
-      <c r="F37" t="n">
-        <v>19.65</v>
-      </c>
-      <c r="G37" t="n">
-        <v>20</v>
+        <v>23.33</v>
       </c>
     </row>
     <row r="38">
@@ -1432,22 +1329,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>21.43</v>
+        <v>38.21</v>
       </c>
       <c r="C38" t="n">
-        <v>8.859999999999999</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>18.15</v>
+        <v>17.55</v>
       </c>
       <c r="E38" t="n">
-        <v>31.82</v>
-      </c>
-      <c r="F38" t="n">
-        <v>19.74</v>
-      </c>
-      <c r="G38" t="n">
-        <v>20</v>
+        <v>24.24</v>
       </c>
     </row>
     <row r="39">
@@ -1455,22 +1346,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>21.36</v>
+        <v>37.65</v>
       </c>
       <c r="C39" t="n">
-        <v>8.69</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>17.8</v>
+        <v>17.22</v>
       </c>
       <c r="E39" t="n">
-        <v>32.22</v>
-      </c>
-      <c r="F39" t="n">
-        <v>19.93</v>
-      </c>
-      <c r="G39" t="n">
-        <v>20.36666666666667</v>
+        <v>25.13</v>
       </c>
     </row>
     <row r="40">
@@ -1478,22 +1363,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>21.29</v>
+        <v>36.82</v>
       </c>
       <c r="C40" t="n">
-        <v>8.550000000000001</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>17.44</v>
+        <v>16.87</v>
       </c>
       <c r="E40" t="n">
-        <v>32.57</v>
-      </c>
-      <c r="F40" t="n">
-        <v>20.03</v>
-      </c>
-      <c r="G40" t="n">
-        <v>20.55</v>
+        <v>26.31</v>
       </c>
     </row>
     <row r="41">
@@ -1501,22 +1380,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>21.22</v>
+        <v>35.94</v>
       </c>
       <c r="C41" t="n">
-        <v>8.65</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>17.11</v>
+        <v>16.52</v>
       </c>
       <c r="E41" t="n">
-        <v>32.65</v>
-      </c>
-      <c r="F41" t="n">
-        <v>20.15</v>
-      </c>
-      <c r="G41" t="n">
-        <v>20.48</v>
+        <v>27.54</v>
       </c>
     </row>
     <row r="42">
@@ -1524,22 +1397,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20.99</v>
+        <v>34.99</v>
       </c>
       <c r="C42" t="n">
-        <v>8.75</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>16.71</v>
+        <v>16.57</v>
       </c>
       <c r="E42" t="n">
-        <v>33.05</v>
-      </c>
-      <c r="F42" t="n">
-        <v>20.27</v>
-      </c>
-      <c r="G42" t="n">
-        <v>19.14166666666667</v>
+        <v>28.44</v>
       </c>
     </row>
     <row r="43">
@@ -1547,22 +1414,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20.8</v>
+        <v>34.79</v>
       </c>
       <c r="C43" t="n">
-        <v>8.779999999999999</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>16.07</v>
+        <v>16.6</v>
       </c>
       <c r="E43" t="n">
-        <v>34.47</v>
-      </c>
-      <c r="F43" t="n">
-        <v>20.39</v>
-      </c>
-      <c r="G43" t="n">
-        <v>18.87857142857143</v>
+        <v>28.61</v>
       </c>
     </row>
     <row r="44">
@@ -1570,22 +1431,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20.69</v>
+        <v>34.56</v>
       </c>
       <c r="C44" t="n">
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>15.43</v>
+        <v>16.64</v>
       </c>
       <c r="E44" t="n">
-        <v>35.64</v>
-      </c>
-      <c r="F44" t="n">
-        <v>20.53</v>
-      </c>
-      <c r="G44" t="n">
-        <v>18.89375</v>
+        <v>28.79</v>
       </c>
     </row>
     <row r="45">
@@ -1593,22 +1448,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20.57</v>
+        <v>34.34</v>
       </c>
       <c r="C45" t="n">
-        <v>8.33</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>14.72</v>
+        <v>16.73</v>
       </c>
       <c r="E45" t="n">
-        <v>36.8</v>
-      </c>
-      <c r="F45" t="n">
-        <v>20.46</v>
-      </c>
-      <c r="G45" t="n">
-        <v>19.88888888888889</v>
+        <v>28.95</v>
       </c>
     </row>
     <row r="46">
@@ -1616,22 +1465,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20.45</v>
+        <v>34.11</v>
       </c>
       <c r="C46" t="n">
-        <v>7.52</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>13.76</v>
+        <v>16.83</v>
       </c>
       <c r="E46" t="n">
-        <v>38.01</v>
-      </c>
-      <c r="F46" t="n">
-        <v>20.36</v>
-      </c>
-      <c r="G46" t="n">
-        <v>20.665</v>
+        <v>29.11</v>
       </c>
     </row>
     <row r="47">
@@ -1639,22 +1482,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20.3</v>
+        <v>33.79</v>
       </c>
       <c r="C47" t="n">
-        <v>6.72</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>12.83</v>
+        <v>16.96</v>
       </c>
       <c r="E47" t="n">
-        <v>39.19</v>
-      </c>
-      <c r="F47" t="n">
-        <v>20.3</v>
-      </c>
-      <c r="G47" t="n">
-        <v>20.665</v>
+        <v>29.31</v>
       </c>
     </row>
     <row r="48">
@@ -1662,22 +1499,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20.21</v>
+        <v>33.48</v>
       </c>
       <c r="C48" t="n">
-        <v>7.92</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>11.88</v>
+        <v>17.06</v>
       </c>
       <c r="E48" t="n">
-        <v>40.39</v>
-      </c>
-      <c r="F48" t="n">
-        <v>20.24</v>
-      </c>
-      <c r="G48" t="n">
-        <v>21.358</v>
+        <v>29.54</v>
       </c>
     </row>
     <row r="49">
@@ -1685,22 +1516,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20.1</v>
+        <v>33.24</v>
       </c>
       <c r="C49" t="n">
-        <v>9.16</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>10.92</v>
+        <v>17.06</v>
       </c>
       <c r="E49" t="n">
-        <v>41.55</v>
-      </c>
-      <c r="F49" t="n">
-        <v>20.16</v>
-      </c>
-      <c r="G49" t="n">
-        <v>22.111</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="50">
@@ -1708,22 +1533,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>19.97</v>
+        <v>33.27</v>
       </c>
       <c r="C50" t="n">
-        <v>10.38</v>
+        <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>9.960000000000001</v>
+        <v>17.26</v>
       </c>
       <c r="E50" t="n">
-        <v>42.78</v>
-      </c>
-      <c r="F50" t="n">
-        <v>20.15000000000001</v>
-      </c>
-      <c r="G50" t="n">
-        <v>22.754</v>
+        <v>29.59</v>
       </c>
     </row>
     <row r="51">
@@ -1731,22 +1550,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>19.84</v>
+        <v>33.3</v>
       </c>
       <c r="C51" t="n">
-        <v>11.27</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>9</v>
+        <v>17.47</v>
       </c>
       <c r="E51" t="n">
-        <v>44.2</v>
-      </c>
-      <c r="F51" t="n">
-        <v>20.14</v>
-      </c>
-      <c r="G51" t="n">
-        <v>23.547</v>
+        <v>29.37</v>
       </c>
     </row>
     <row r="52">
@@ -1754,22 +1567,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>19.71</v>
+        <v>33.4</v>
       </c>
       <c r="C52" t="n">
-        <v>12.2</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>8.130000000000001</v>
+        <v>17.61</v>
       </c>
       <c r="E52" t="n">
-        <v>45.41</v>
-      </c>
-      <c r="F52" t="n">
-        <v>20.12</v>
-      </c>
-      <c r="G52" t="n">
-        <v>24.43</v>
+        <v>29.15</v>
       </c>
     </row>
     <row r="53">
@@ -1777,22 +1584,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>19.58</v>
+        <v>33.4</v>
       </c>
       <c r="C53" t="n">
-        <v>13.13</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>7.71</v>
+        <v>17.46</v>
       </c>
       <c r="E53" t="n">
-        <v>45.47</v>
-      </c>
-      <c r="F53" t="n">
-        <v>20.1</v>
-      </c>
-      <c r="G53" t="n">
-        <v>26.008</v>
+        <v>29.32</v>
       </c>
     </row>
     <row r="54">
@@ -1800,22 +1601,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>19.45</v>
+        <v>33.4</v>
       </c>
       <c r="C54" t="n">
-        <v>14.37</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>7.29</v>
+        <v>17.34</v>
       </c>
       <c r="E54" t="n">
-        <v>45.53</v>
-      </c>
-      <c r="F54" t="n">
-        <v>20.08</v>
-      </c>
-      <c r="G54" t="n">
-        <v>27.28100000000001</v>
+        <v>29.46</v>
       </c>
     </row>
     <row r="55">
@@ -1823,22 +1618,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>19.33</v>
+        <v>33.4</v>
       </c>
       <c r="C55" t="n">
-        <v>15.68</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>6.84</v>
+        <v>17.2</v>
       </c>
       <c r="E55" t="n">
-        <v>44.68</v>
-      </c>
-      <c r="F55" t="n">
-        <v>20</v>
-      </c>
-      <c r="G55" t="n">
-        <v>29.46400000000001</v>
+        <v>29.6</v>
       </c>
     </row>
     <row r="56">
@@ -1846,22 +1635,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>19.21</v>
+        <v>33.4</v>
       </c>
       <c r="C56" t="n">
-        <v>17.87</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>6.65</v>
+        <v>17.04</v>
       </c>
       <c r="E56" t="n">
-        <v>43.7</v>
-      </c>
-      <c r="F56" t="n">
-        <v>19.94</v>
-      </c>
-      <c r="G56" t="n">
-        <v>30.632</v>
+        <v>29.76</v>
       </c>
     </row>
     <row r="57">
@@ -1869,22 +1652,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>19.08</v>
+        <v>33.4</v>
       </c>
       <c r="C57" t="n">
-        <v>20.06</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>6.45</v>
+        <v>16.91</v>
       </c>
       <c r="E57" t="n">
-        <v>42.51</v>
-      </c>
-      <c r="F57" t="n">
-        <v>19.82</v>
-      </c>
-      <c r="G57" t="n">
-        <v>32.08499999999999</v>
+        <v>29.89</v>
       </c>
     </row>
     <row r="58">
@@ -1892,22 +1669,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>18.87</v>
+        <v>33.4</v>
       </c>
       <c r="C58" t="n">
-        <v>20.23</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>6.51</v>
+        <v>16.71</v>
       </c>
       <c r="E58" t="n">
-        <v>40.91</v>
-      </c>
-      <c r="F58" t="n">
-        <v>19.874</v>
-      </c>
-      <c r="G58" t="n">
-        <v>33.60999999999999</v>
+        <v>30.09</v>
       </c>
     </row>
     <row r="59">
@@ -1915,22 +1686,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>18.65</v>
+        <v>33.4</v>
       </c>
       <c r="C59" t="n">
-        <v>20.48</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>6.59</v>
+        <v>16.57</v>
       </c>
       <c r="E59" t="n">
-        <v>39.33</v>
-      </c>
-      <c r="F59" t="n">
-        <v>19.908</v>
-      </c>
-      <c r="G59" t="n">
-        <v>35.05499999999999</v>
+        <v>30.23</v>
       </c>
     </row>
     <row r="60">
@@ -1938,22 +1703,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>18.46</v>
+        <v>33.4</v>
       </c>
       <c r="C60" t="n">
-        <v>20.75</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>6.74</v>
+        <v>16.18</v>
       </c>
       <c r="E60" t="n">
-        <v>37.75</v>
-      </c>
-      <c r="F60" t="n">
-        <v>19.872</v>
-      </c>
-      <c r="G60" t="n">
-        <v>36.45</v>
+        <v>30.62</v>
       </c>
     </row>
     <row r="61">
@@ -1961,22 +1720,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>18.27</v>
+        <v>33.4</v>
       </c>
       <c r="C61" t="n">
-        <v>21.04</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>6.88</v>
+        <v>15.83</v>
       </c>
       <c r="E61" t="n">
-        <v>36.27</v>
-      </c>
-      <c r="F61" t="n">
-        <v>19.856</v>
-      </c>
-      <c r="G61" t="n">
-        <v>37.69500000000001</v>
+        <v>30.97</v>
       </c>
     </row>
     <row r="62">
@@ -1984,22 +1737,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>18.07</v>
+        <v>33.4</v>
       </c>
       <c r="C62" t="n">
-        <v>20.96</v>
+        <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>7.02</v>
+        <v>15.53</v>
       </c>
       <c r="E62" t="n">
-        <v>33.96</v>
-      </c>
-      <c r="F62" t="n">
-        <v>19.85</v>
-      </c>
-      <c r="G62" t="n">
-        <v>40.16</v>
+        <v>31.27</v>
       </c>
     </row>
     <row r="63">
@@ -2007,22 +1754,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>17.86</v>
+        <v>33.4</v>
       </c>
       <c r="C63" t="n">
-        <v>20.9</v>
+        <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>6.98</v>
+        <v>15.56</v>
       </c>
       <c r="E63" t="n">
-        <v>31.76</v>
-      </c>
-      <c r="F63" t="n">
-        <v>19.824</v>
-      </c>
-      <c r="G63" t="n">
-        <v>42.705</v>
+        <v>31.24</v>
       </c>
     </row>
     <row r="64">
@@ -2030,22 +1771,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>17.64</v>
+        <v>33.4</v>
       </c>
       <c r="C64" t="n">
-        <v>20.9</v>
+        <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>6.96</v>
+        <v>15.55</v>
       </c>
       <c r="E64" t="n">
-        <v>29.63</v>
-      </c>
-      <c r="F64" t="n">
-        <v>19.718</v>
-      </c>
-      <c r="G64" t="n">
-        <v>45.17</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="65">
@@ -2053,22 +1788,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>17.43</v>
+        <v>33.4</v>
       </c>
       <c r="C65" t="n">
-        <v>20.89</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>7.02</v>
+        <v>15.46</v>
       </c>
       <c r="E65" t="n">
-        <v>28.43</v>
-      </c>
-      <c r="F65" t="n">
-        <v>19.692</v>
-      </c>
-      <c r="G65" t="n">
-        <v>46.56500000000001</v>
+        <v>31.34</v>
       </c>
     </row>
     <row r="66">
@@ -2076,22 +1805,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>17.23</v>
+        <v>33.4</v>
       </c>
       <c r="C66" t="n">
-        <v>20.5</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>7.06</v>
+        <v>15.27</v>
       </c>
       <c r="E66" t="n">
-        <v>27.35</v>
-      </c>
-      <c r="F66" t="n">
-        <v>19.606</v>
-      </c>
-      <c r="G66" t="n">
-        <v>48.27</v>
+        <v>31.53</v>
       </c>
     </row>
     <row r="67">
@@ -2099,22 +1822,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>17.05</v>
+        <v>33.4</v>
       </c>
       <c r="C67" t="n">
-        <v>20.11</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>7.09</v>
+        <v>15.09</v>
       </c>
       <c r="E67" t="n">
-        <v>26.64</v>
-      </c>
-      <c r="F67" t="n">
-        <v>19.54</v>
-      </c>
-      <c r="G67" t="n">
-        <v>49.59000000000001</v>
+        <v>31.71</v>
       </c>
     </row>
     <row r="68">
@@ -2122,22 +1839,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>17</v>
+        <v>33.4</v>
       </c>
       <c r="C68" t="n">
-        <v>19.77</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>7.12</v>
+        <v>14.98</v>
       </c>
       <c r="E68" t="n">
-        <v>25.92</v>
-      </c>
-      <c r="F68" t="n">
-        <v>19.3</v>
-      </c>
-      <c r="G68" t="n">
-        <v>50.91000000000001</v>
+        <v>31.82</v>
       </c>
     </row>
     <row r="69">
@@ -2145,22 +1856,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>16.94</v>
+        <v>33.4</v>
       </c>
       <c r="C69" t="n">
-        <v>19.35</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>7.15</v>
+        <v>14.84</v>
       </c>
       <c r="E69" t="n">
-        <v>25.2</v>
-      </c>
-      <c r="F69" t="n">
-        <v>19.07999999999999</v>
-      </c>
-      <c r="G69" t="n">
-        <v>52.27999999999999</v>
+        <v>31.96</v>
       </c>
     </row>
     <row r="70">
@@ -2168,22 +1873,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>16.88</v>
+        <v>33.4</v>
       </c>
       <c r="C70" t="n">
-        <v>18.87</v>
+        <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>7.11</v>
+        <v>14.77</v>
       </c>
       <c r="E70" t="n">
-        <v>24.5</v>
-      </c>
-      <c r="F70" t="n">
-        <v>18.87</v>
-      </c>
-      <c r="G70" t="n">
-        <v>53.77</v>
+        <v>32.03</v>
       </c>
     </row>
     <row r="71">
@@ -2191,22 +1890,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>16.82</v>
+        <v>33.4</v>
       </c>
       <c r="C71" t="n">
-        <v>18.37</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>7.08</v>
+        <v>14.62</v>
       </c>
       <c r="E71" t="n">
-        <v>23.45</v>
-      </c>
-      <c r="F71" t="n">
-        <v>19.04</v>
-      </c>
-      <c r="G71" t="n">
-        <v>55.23999999999999</v>
+        <v>32.18</v>
       </c>
     </row>
     <row r="72">
@@ -2214,22 +1907,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>16.78</v>
+        <v>33.4</v>
       </c>
       <c r="C72" t="n">
-        <v>18.21</v>
+        <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>7.09</v>
+        <v>14.42</v>
       </c>
       <c r="E72" t="n">
-        <v>23.26</v>
-      </c>
-      <c r="F72" t="n">
-        <v>19.13</v>
-      </c>
-      <c r="G72" t="n">
-        <v>55.52999999999999</v>
+        <v>32.38</v>
       </c>
     </row>
     <row r="73">
@@ -2237,22 +1924,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>16.75</v>
+        <v>33.4</v>
       </c>
       <c r="C73" t="n">
-        <v>18.35</v>
+        <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>6.96</v>
+        <v>14.22</v>
       </c>
       <c r="E73" t="n">
-        <v>23.02</v>
-      </c>
-      <c r="F73" t="n">
-        <v>19.22</v>
-      </c>
-      <c r="G73" t="n">
-        <v>55.69999999999999</v>
+        <v>32.58</v>
       </c>
     </row>
     <row r="74">
@@ -2260,22 +1941,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>16.64</v>
+        <v>33.4</v>
       </c>
       <c r="C74" t="n">
-        <v>18.51</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>6.83</v>
+        <v>14.05</v>
       </c>
       <c r="E74" t="n">
-        <v>22.6</v>
-      </c>
-      <c r="F74" t="n">
-        <v>19.66</v>
-      </c>
-      <c r="G74" t="n">
-        <v>55.77</v>
+        <v>32.75</v>
       </c>
     </row>
     <row r="75">
@@ -2283,22 +1958,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>16.51</v>
+        <v>33.4</v>
       </c>
       <c r="C75" t="n">
-        <v>18.68</v>
+        <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>6.68</v>
+        <v>13.92</v>
       </c>
       <c r="E75" t="n">
-        <v>22.22</v>
-      </c>
-      <c r="F75" t="n">
-        <v>20.08</v>
-      </c>
-      <c r="G75" t="n">
-        <v>55.83000000000001</v>
+        <v>32.88</v>
       </c>
     </row>
     <row r="76">
@@ -2306,22 +1975,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>16.39</v>
+        <v>33.4</v>
       </c>
       <c r="C76" t="n">
-        <v>18.85</v>
+        <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>6.6</v>
+        <v>13.92</v>
       </c>
       <c r="E76" t="n">
-        <v>21.84</v>
-      </c>
-      <c r="F76" t="n">
-        <v>20.57</v>
-      </c>
-      <c r="G76" t="n">
-        <v>55.75500000000001</v>
+        <v>32.88</v>
       </c>
     </row>
     <row r="77">
@@ -2329,22 +1992,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>16.26</v>
+        <v>33.4</v>
       </c>
       <c r="C77" t="n">
-        <v>18.43</v>
+        <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>7.29</v>
+        <v>13.99</v>
       </c>
       <c r="E77" t="n">
-        <v>21.26</v>
-      </c>
-      <c r="F77" t="n">
-        <v>21.04</v>
-      </c>
-      <c r="G77" t="n">
-        <v>55.72000000000001</v>
+        <v>32.81</v>
       </c>
     </row>
     <row r="78">
@@ -2352,22 +2009,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>16.16</v>
+        <v>33.4</v>
       </c>
       <c r="C78" t="n">
-        <v>17.92</v>
+        <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>7.96</v>
+        <v>14.06</v>
       </c>
       <c r="E78" t="n">
-        <v>20.66</v>
-      </c>
-      <c r="F78" t="n">
-        <v>21.635</v>
-      </c>
-      <c r="G78" t="n">
-        <v>55.665</v>
+        <v>32.74</v>
       </c>
     </row>
     <row r="79">
@@ -2375,22 +2026,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>16.37</v>
+        <v>33.4</v>
       </c>
       <c r="C79" t="n">
-        <v>17.35</v>
+        <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>8.630000000000001</v>
+        <v>14.13</v>
       </c>
       <c r="E79" t="n">
-        <v>19.83</v>
-      </c>
-      <c r="F79" t="n">
-        <v>22.25</v>
-      </c>
-      <c r="G79" t="n">
-        <v>55.58</v>
+        <v>32.67</v>
       </c>
     </row>
     <row r="80">
@@ -2398,22 +2043,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>16.55</v>
+        <v>33.4</v>
       </c>
       <c r="C80" t="n">
-        <v>16.85</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>9.300000000000001</v>
+        <v>14.21</v>
       </c>
       <c r="E80" t="n">
-        <v>18.92</v>
-      </c>
-      <c r="F80" t="n">
-        <v>22.875</v>
-      </c>
-      <c r="G80" t="n">
-        <v>55.525</v>
+        <v>32.59</v>
       </c>
     </row>
     <row r="81">
@@ -2421,22 +2060,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>16.74</v>
+        <v>33.4</v>
       </c>
       <c r="C81" t="n">
-        <v>16.36</v>
+        <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>9.960000000000001</v>
+        <v>14.37</v>
       </c>
       <c r="E81" t="n">
-        <v>18.35</v>
-      </c>
-      <c r="F81" t="n">
-        <v>23.13</v>
-      </c>
-      <c r="G81" t="n">
-        <v>55.48999999999999</v>
+        <v>32.43</v>
       </c>
     </row>
     <row r="82">
@@ -2444,22 +2077,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>16.91</v>
+        <v>33.4</v>
       </c>
       <c r="C82" t="n">
-        <v>15.87</v>
+        <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>10.46</v>
+        <v>14.7</v>
       </c>
       <c r="E82" t="n">
-        <v>17.75</v>
-      </c>
-      <c r="F82" t="n">
-        <v>23.455</v>
-      </c>
-      <c r="G82" t="n">
-        <v>55.565</v>
+        <v>32.1</v>
       </c>
     </row>
     <row r="83">
@@ -2467,22 +2094,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>17.09</v>
+        <v>33.4</v>
       </c>
       <c r="C83" t="n">
-        <v>15.08</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>11.08</v>
+        <v>14.99</v>
       </c>
       <c r="E83" t="n">
-        <v>17.18</v>
-      </c>
-      <c r="F83" t="n">
-        <v>23.84</v>
-      </c>
-      <c r="G83" t="n">
-        <v>55.73999999999999</v>
+        <v>31.81</v>
       </c>
     </row>
     <row r="84">
@@ -2490,22 +2111,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>17.36</v>
+        <v>33.4</v>
       </c>
       <c r="C84" t="n">
-        <v>14.26</v>
+        <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>11.69</v>
+        <v>15.28</v>
       </c>
       <c r="E84" t="n">
-        <v>16.77</v>
-      </c>
-      <c r="F84" t="n">
-        <v>23.935</v>
-      </c>
-      <c r="G84" t="n">
-        <v>55.99499999999999</v>
+        <v>31.52</v>
       </c>
     </row>
     <row r="85">
@@ -2513,22 +2128,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>17.67</v>
+        <v>33.4</v>
       </c>
       <c r="C85" t="n">
-        <v>13.45</v>
+        <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>12.3</v>
+        <v>15.58</v>
       </c>
       <c r="E85" t="n">
-        <v>16.29</v>
-      </c>
-      <c r="F85" t="n">
-        <v>24.05</v>
-      </c>
-      <c r="G85" t="n">
-        <v>56.25</v>
+        <v>31.22</v>
       </c>
     </row>
     <row r="86">
@@ -2536,22 +2145,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>17.98</v>
+        <v>33.4</v>
       </c>
       <c r="C86" t="n">
-        <v>11.48</v>
+        <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>12.87</v>
+        <v>15.85</v>
       </c>
       <c r="E86" t="n">
-        <v>15.76</v>
-      </c>
-      <c r="F86" t="n">
-        <v>24.155</v>
-      </c>
-      <c r="G86" t="n">
-        <v>57.779</v>
+        <v>30.95</v>
       </c>
     </row>
     <row r="87">
@@ -2559,22 +2162,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>18.29</v>
+        <v>33.4</v>
       </c>
       <c r="C87" t="n">
-        <v>10.09</v>
+        <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>12.67</v>
+        <v>16.08</v>
       </c>
       <c r="E87" t="n">
-        <v>15.28</v>
-      </c>
-      <c r="F87" t="n">
-        <v>24.27</v>
-      </c>
-      <c r="G87" t="n">
-        <v>59.41800000000001</v>
+        <v>30.72</v>
       </c>
     </row>
     <row r="88">
@@ -2582,22 +2179,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>18.59</v>
+        <v>33.4</v>
       </c>
       <c r="C88" t="n">
-        <v>8.77</v>
+        <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>12.49</v>
+        <v>16.31</v>
       </c>
       <c r="E88" t="n">
-        <v>14.81</v>
-      </c>
-      <c r="F88" t="n">
-        <v>24.26</v>
-      </c>
-      <c r="G88" t="n">
-        <v>61.097</v>
+        <v>30.49</v>
       </c>
     </row>
     <row r="89">
@@ -2605,22 +2196,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>18.57</v>
+        <v>33.4</v>
       </c>
       <c r="C89" t="n">
-        <v>9.51</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>12.31</v>
+        <v>16.66</v>
       </c>
       <c r="E89" t="n">
-        <v>14.49</v>
-      </c>
-      <c r="F89" t="n">
-        <v>24.23</v>
-      </c>
-      <c r="G89" t="n">
-        <v>62.89600000000002</v>
+        <v>30.14</v>
       </c>
     </row>
     <row r="90">
@@ -2628,22 +2213,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>18.56</v>
+        <v>33.4</v>
       </c>
       <c r="C90" t="n">
-        <v>10.25</v>
+        <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>12.1</v>
+        <v>17</v>
       </c>
       <c r="E90" t="n">
-        <v>14.32</v>
-      </c>
-      <c r="F90" t="n">
-        <v>24.18</v>
-      </c>
-      <c r="G90" t="n">
-        <v>64.59500000000001</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="91">
@@ -2651,22 +2230,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>18.54</v>
+        <v>33.4</v>
       </c>
       <c r="C91" t="n">
-        <v>10.97</v>
+        <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>11.9</v>
+        <v>16.95</v>
       </c>
       <c r="E91" t="n">
-        <v>14.2</v>
-      </c>
-      <c r="F91" t="n">
-        <v>24.1</v>
-      </c>
-      <c r="G91" t="n">
-        <v>66.29400000000001</v>
+        <v>29.86</v>
       </c>
     </row>
     <row r="92">
@@ -2674,25 +2247,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>18.52</v>
+        <v>33.4</v>
       </c>
       <c r="C92" t="n">
-        <v>11.29</v>
+        <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>11.82</v>
+        <v>16.75</v>
       </c>
       <c r="E92" t="n">
-        <v>14</v>
-      </c>
-      <c r="F92" t="n">
-        <v>24.01</v>
-      </c>
-      <c r="G92" t="n">
-        <v>68.36299999999999</v>
-      </c>
-      <c r="H92" t="n">
-        <v>10</v>
+        <v>30.05</v>
       </c>
     </row>
     <row r="93">
@@ -2700,25 +2264,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>18.48</v>
+        <v>33.4</v>
       </c>
       <c r="C93" t="n">
-        <v>11.6</v>
+        <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>11.74</v>
+        <v>16.57</v>
       </c>
       <c r="E93" t="n">
-        <v>13.68</v>
-      </c>
-      <c r="F93" t="n">
-        <v>23.86</v>
-      </c>
-      <c r="G93" t="n">
-        <v>70.63199999999998</v>
-      </c>
-      <c r="H93" t="n">
-        <v>9.715</v>
+        <v>30.24</v>
       </c>
     </row>
     <row r="94">
@@ -2726,25 +2281,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>18.38</v>
+        <v>33.4</v>
       </c>
       <c r="C94" t="n">
-        <v>11.95</v>
+        <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>11.53</v>
+        <v>16.38</v>
       </c>
       <c r="E94" t="n">
-        <v>13.64</v>
-      </c>
-      <c r="F94" t="n">
-        <v>23.73</v>
-      </c>
-      <c r="G94" t="n">
-        <v>72.821</v>
-      </c>
-      <c r="H94" t="n">
-        <v>9.619999999999999</v>
+        <v>30.42</v>
       </c>
     </row>
     <row r="95">
@@ -2752,25 +2298,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>18.19</v>
+        <v>33.4</v>
       </c>
       <c r="C95" t="n">
-        <v>12.3</v>
+        <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>11.35</v>
+        <v>16.02</v>
       </c>
       <c r="E95" t="n">
-        <v>13.67</v>
-      </c>
-      <c r="F95" t="n">
-        <v>23.6</v>
-      </c>
-      <c r="G95" t="n">
-        <v>75.00999999999999</v>
-      </c>
-      <c r="H95" t="n">
-        <v>7.215</v>
+        <v>30.78</v>
       </c>
     </row>
     <row r="96">
@@ -2778,25 +2315,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>19.1</v>
+        <v>33.4</v>
       </c>
       <c r="C96" t="n">
-        <v>13.88</v>
+        <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>11.16</v>
+        <v>15.87</v>
       </c>
       <c r="E96" t="n">
-        <v>13.76</v>
-      </c>
-      <c r="F96" t="n">
-        <v>23.41</v>
-      </c>
-      <c r="G96" t="n">
-        <v>75.88</v>
-      </c>
-      <c r="H96" t="n">
-        <v>9.772</v>
+        <v>30.93</v>
       </c>
     </row>
     <row r="97">
@@ -2804,25 +2332,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>20.02</v>
+        <v>33.4</v>
       </c>
       <c r="C97" t="n">
-        <v>15.61</v>
+        <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>10.97</v>
+        <v>15.72</v>
       </c>
       <c r="E97" t="n">
-        <v>13.79</v>
-      </c>
-      <c r="F97" t="n">
-        <v>23.22</v>
-      </c>
-      <c r="G97" t="n">
-        <v>76.57999999999998</v>
-      </c>
-      <c r="H97" t="n">
-        <v>11.34333333333333</v>
+        <v>31.09</v>
       </c>
     </row>
     <row r="98">
@@ -2830,25 +2349,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>20.93</v>
+        <v>33.4</v>
       </c>
       <c r="C98" t="n">
-        <v>17.33</v>
+        <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>10.79</v>
+        <v>15.56</v>
       </c>
       <c r="E98" t="n">
-        <v>13.52</v>
-      </c>
-      <c r="F98" t="n">
-        <v>23.03</v>
-      </c>
-      <c r="G98" t="n">
-        <v>77.67999999999999</v>
-      </c>
-      <c r="H98" t="n">
-        <v>12.43714285714286</v>
+        <v>31.24</v>
       </c>
     </row>
     <row r="99">
@@ -2856,25 +2366,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>21.87</v>
+        <v>33.4</v>
       </c>
       <c r="C99" t="n">
-        <v>17.05</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>10.6</v>
+        <v>16.35</v>
       </c>
       <c r="E99" t="n">
-        <v>14.14</v>
-      </c>
-      <c r="F99" t="n">
-        <v>22.84</v>
-      </c>
-      <c r="G99" t="n">
-        <v>77.88</v>
-      </c>
-      <c r="H99" t="n">
-        <v>13.2575</v>
+        <v>30.46</v>
       </c>
     </row>
     <row r="100">
@@ -2882,25 +2383,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>22.82</v>
+        <v>33.4</v>
       </c>
       <c r="C100" t="n">
-        <v>17.16</v>
+        <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>10.42</v>
+        <v>17.2</v>
       </c>
       <c r="E100" t="n">
-        <v>14.33</v>
-      </c>
-      <c r="F100" t="n">
-        <v>22.67</v>
-      </c>
-      <c r="G100" t="n">
-        <v>78.06999999999998</v>
-      </c>
-      <c r="H100" t="n">
-        <v>13.89555555555556</v>
+        <v>29.6</v>
       </c>
     </row>
     <row r="101">
@@ -2908,25 +2400,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>23.78</v>
+        <v>33.4</v>
       </c>
       <c r="C101" t="n">
-        <v>17.26</v>
+        <v>0</v>
       </c>
       <c r="D101" t="n">
-        <v>10.22</v>
+        <v>18.49</v>
       </c>
       <c r="E101" t="n">
-        <v>14.53</v>
-      </c>
-      <c r="F101" t="n">
-        <v>22.52</v>
-      </c>
-      <c r="G101" t="n">
-        <v>78.25999999999999</v>
-      </c>
-      <c r="H101" t="n">
-        <v>14.406</v>
+        <v>28.31</v>
       </c>
     </row>
     <row r="102">
@@ -2934,25 +2417,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>24.73</v>
+        <v>33.4</v>
       </c>
       <c r="C102" t="n">
-        <v>17.79</v>
+        <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>10.03</v>
+        <v>19.56</v>
       </c>
       <c r="E102" t="n">
-        <v>14.81</v>
-      </c>
-      <c r="F102" t="n">
-        <v>22.39</v>
-      </c>
-      <c r="G102" t="n">
-        <v>77.92999999999999</v>
-      </c>
-      <c r="H102" t="n">
-        <v>14.406</v>
+        <v>27.24</v>
       </c>
     </row>
     <row r="103">
@@ -2960,25 +2434,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>25.68</v>
+        <v>33.4</v>
       </c>
       <c r="C103" t="n">
-        <v>18.2</v>
+        <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>9.85</v>
+        <v>20.46</v>
       </c>
       <c r="E103" t="n">
-        <v>15.38</v>
-      </c>
-      <c r="F103" t="n">
-        <v>22.26</v>
-      </c>
-      <c r="G103" t="n">
-        <v>77.41999999999999</v>
-      </c>
-      <c r="H103" t="n">
-        <v>15.286</v>
+        <v>26.34</v>
       </c>
     </row>
     <row r="104">
@@ -2986,25 +2451,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>28.24</v>
+        <v>33.4</v>
       </c>
       <c r="C104" t="n">
-        <v>17.28</v>
+        <v>0</v>
       </c>
       <c r="D104" t="n">
-        <v>9.73</v>
+        <v>21.43</v>
       </c>
       <c r="E104" t="n">
-        <v>15.62</v>
-      </c>
-      <c r="F104" t="n">
-        <v>22.11</v>
-      </c>
-      <c r="G104" t="n">
-        <v>76.91</v>
-      </c>
-      <c r="H104" t="n">
-        <v>16.203</v>
+        <v>25.37</v>
       </c>
     </row>
     <row r="105">
@@ -3012,25 +2468,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>30.85</v>
+        <v>33.4</v>
       </c>
       <c r="C105" t="n">
-        <v>16.34</v>
+        <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>9.609999999999999</v>
+        <v>22.57</v>
       </c>
       <c r="E105" t="n">
-        <v>15.79</v>
-      </c>
-      <c r="F105" t="n">
-        <v>21.96</v>
-      </c>
-      <c r="G105" t="n">
-        <v>76.42999999999999</v>
-      </c>
-      <c r="H105" t="n">
-        <v>17.1</v>
+        <v>24.23</v>
       </c>
     </row>
     <row r="106">
@@ -3038,25 +2485,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>31.72</v>
+        <v>33.4</v>
       </c>
       <c r="C106" t="n">
-        <v>15.35</v>
+        <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>9.49</v>
+        <v>23.47</v>
       </c>
       <c r="E106" t="n">
-        <v>15.96</v>
-      </c>
-      <c r="F106" t="n">
-        <v>21.89</v>
-      </c>
-      <c r="G106" t="n">
-        <v>76.654</v>
-      </c>
-      <c r="H106" t="n">
-        <v>18.93</v>
+        <v>23.33</v>
       </c>
     </row>
     <row r="107">
@@ -3064,25 +2502,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>32.54</v>
+        <v>33.4</v>
       </c>
       <c r="C107" t="n">
-        <v>14.21</v>
+        <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>9.35</v>
+        <v>24.37</v>
       </c>
       <c r="E107" t="n">
-        <v>16.22</v>
-      </c>
-      <c r="F107" t="n">
-        <v>21.83000000000001</v>
-      </c>
-      <c r="G107" t="n">
-        <v>77.15200000000002</v>
-      </c>
-      <c r="H107" t="n">
-        <v>18.703</v>
+        <v>22.43</v>
       </c>
     </row>
     <row r="108">
@@ -3090,25 +2519,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>33.35</v>
+        <v>33.4</v>
       </c>
       <c r="C108" t="n">
-        <v>12.99</v>
+        <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>9.199999999999999</v>
+        <v>25.32</v>
       </c>
       <c r="E108" t="n">
-        <v>16.73</v>
-      </c>
-      <c r="F108" t="n">
-        <v>21.67000000000001</v>
-      </c>
-      <c r="G108" t="n">
-        <v>77.52000000000001</v>
-      </c>
-      <c r="H108" t="n">
-        <v>18.536</v>
+        <v>21.48</v>
       </c>
     </row>
     <row r="109">
@@ -3116,25 +2536,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>34.09</v>
+        <v>33.38</v>
       </c>
       <c r="C109" t="n">
-        <v>11.78</v>
+        <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>9.050000000000001</v>
+        <v>25.21</v>
       </c>
       <c r="E109" t="n">
-        <v>16.33</v>
-      </c>
-      <c r="F109" t="n">
-        <v>21.53</v>
-      </c>
-      <c r="G109" t="n">
-        <v>78.828</v>
-      </c>
-      <c r="H109" t="n">
-        <v>18.389</v>
+        <v>21.59</v>
       </c>
     </row>
     <row r="110">
@@ -3142,25 +2553,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>34.82</v>
+        <v>33.52</v>
       </c>
       <c r="C110" t="n">
-        <v>10.18</v>
+        <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>8.92</v>
+        <v>24.86</v>
       </c>
       <c r="E110" t="n">
-        <v>16.35</v>
-      </c>
-      <c r="F110" t="n">
-        <v>21.37</v>
-      </c>
-      <c r="G110" t="n">
-        <v>80.146</v>
-      </c>
-      <c r="H110" t="n">
-        <v>18.222</v>
+        <v>21.78</v>
       </c>
     </row>
     <row r="111">
@@ -3168,25 +2570,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>35.54</v>
+        <v>33.66</v>
       </c>
       <c r="C111" t="n">
-        <v>8.869999999999999</v>
+        <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>8.81</v>
+        <v>24.44</v>
       </c>
       <c r="E111" t="n">
-        <v>16.23</v>
-      </c>
-      <c r="F111" t="n">
-        <v>21.13</v>
-      </c>
-      <c r="G111" t="n">
-        <v>81.38400000000001</v>
-      </c>
-      <c r="H111" t="n">
-        <v>18.035</v>
+        <v>22.04</v>
       </c>
     </row>
     <row r="112">
@@ -3194,25 +2587,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>36.29</v>
+        <v>33.98</v>
       </c>
       <c r="C112" t="n">
-        <v>7.52</v>
+        <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>8.699999999999999</v>
+        <v>24.11</v>
       </c>
       <c r="E112" t="n">
-        <v>16.06</v>
-      </c>
-      <c r="F112" t="n">
-        <v>20.365</v>
-      </c>
-      <c r="G112" t="n">
-        <v>84.93000000000002</v>
-      </c>
-      <c r="H112" t="n">
-        <v>16.135</v>
+        <v>22.03</v>
       </c>
     </row>
     <row r="113">
@@ -3220,25 +2604,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>37.05</v>
+        <v>34.36</v>
       </c>
       <c r="C113" t="n">
-        <v>6.28</v>
+        <v>0</v>
       </c>
       <c r="D113" t="n">
-        <v>8.59</v>
+        <v>23.9</v>
       </c>
       <c r="E113" t="n">
-        <v>15.47</v>
-      </c>
-      <c r="F113" t="n">
-        <v>19.9</v>
-      </c>
-      <c r="G113" t="n">
-        <v>88.45599999999999</v>
-      </c>
-      <c r="H113" t="n">
-        <v>14.255</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="114">
@@ -3246,25 +2621,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>35.95</v>
+        <v>34.27</v>
       </c>
       <c r="C114" t="n">
-        <v>6.39</v>
+        <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>8.539999999999999</v>
+        <v>24.1</v>
       </c>
       <c r="E114" t="n">
-        <v>15.36</v>
-      </c>
-      <c r="F114" t="n">
-        <v>19.455</v>
-      </c>
-      <c r="G114" t="n">
-        <v>91.91</v>
-      </c>
-      <c r="H114" t="n">
-        <v>14.395</v>
+        <v>21.71</v>
       </c>
     </row>
     <row r="115">
@@ -3272,25 +2638,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>34.86</v>
+        <v>34.36</v>
       </c>
       <c r="C115" t="n">
-        <v>6.46</v>
+        <v>0</v>
       </c>
       <c r="D115" t="n">
-        <v>8.48</v>
+        <v>24.31</v>
       </c>
       <c r="E115" t="n">
-        <v>15.08</v>
-      </c>
-      <c r="F115" t="n">
-        <v>19.23</v>
-      </c>
-      <c r="G115" t="n">
-        <v>95.33399999999999</v>
-      </c>
-      <c r="H115" t="n">
-        <v>14.555</v>
+        <v>21.39</v>
       </c>
     </row>
     <row r="116">
@@ -3298,25 +2655,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>34.39</v>
+        <v>34.75</v>
       </c>
       <c r="C116" t="n">
-        <v>6.59</v>
+        <v>0</v>
       </c>
       <c r="D116" t="n">
-        <v>10.1</v>
+        <v>24.34</v>
       </c>
       <c r="E116" t="n">
-        <v>14.78</v>
-      </c>
-      <c r="F116" t="n">
-        <v>18.186</v>
-      </c>
-      <c r="G116" t="n">
-        <v>98.054</v>
-      </c>
-      <c r="H116" t="n">
-        <v>13.906</v>
+        <v>20.95</v>
       </c>
     </row>
     <row r="117">
@@ -3324,25 +2672,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>33.96</v>
+        <v>35.08</v>
       </c>
       <c r="C117" t="n">
-        <v>6.7</v>
+        <v>0</v>
       </c>
       <c r="D117" t="n">
-        <v>12.37</v>
+        <v>24.29</v>
       </c>
       <c r="E117" t="n">
-        <v>14.19</v>
-      </c>
-      <c r="F117" t="n">
-        <v>16.852</v>
-      </c>
-      <c r="G117" t="n">
-        <v>100.64</v>
-      </c>
-      <c r="H117" t="n">
-        <v>13.294</v>
+        <v>20.65</v>
       </c>
     </row>
     <row r="118">
@@ -3350,25 +2689,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>33.53</v>
+        <v>35.72</v>
       </c>
       <c r="C118" t="n">
-        <v>6.87</v>
+        <v>0</v>
       </c>
       <c r="D118" t="n">
-        <v>14.62</v>
+        <v>23.88</v>
       </c>
       <c r="E118" t="n">
-        <v>13.66</v>
-      </c>
-      <c r="F118" t="n">
-        <v>15.698</v>
-      </c>
-      <c r="G118" t="n">
-        <v>102.936</v>
-      </c>
-      <c r="H118" t="n">
-        <v>12.682</v>
+        <v>20.4</v>
       </c>
     </row>
     <row r="119">
@@ -3376,25 +2706,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>32.7</v>
+        <v>36.18</v>
       </c>
       <c r="C119" t="n">
-        <v>6.95</v>
+        <v>0</v>
       </c>
       <c r="D119" t="n">
-        <v>18.6</v>
+        <v>23.65</v>
       </c>
       <c r="E119" t="n">
-        <v>12.14</v>
-      </c>
-      <c r="F119" t="n">
-        <v>14.544</v>
-      </c>
-      <c r="G119" t="n">
-        <v>105.072</v>
-      </c>
-      <c r="H119" t="n">
-        <v>11.983</v>
+        <v>20.17</v>
       </c>
     </row>
     <row r="120">
@@ -3402,25 +2723,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>32.02</v>
+        <v>36.48</v>
       </c>
       <c r="C120" t="n">
-        <v>7.04</v>
+        <v>0</v>
       </c>
       <c r="D120" t="n">
-        <v>22.58</v>
+        <v>23.64</v>
       </c>
       <c r="E120" t="n">
-        <v>10.58</v>
-      </c>
-      <c r="F120" t="n">
-        <v>13.41</v>
-      </c>
-      <c r="G120" t="n">
-        <v>107.089</v>
-      </c>
-      <c r="H120" t="n">
-        <v>11.294</v>
+        <v>19.88</v>
       </c>
     </row>
     <row r="121">
@@ -3428,25 +2740,16 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>31.27</v>
+        <v>37.12</v>
       </c>
       <c r="C121" t="n">
-        <v>6.86</v>
+        <v>0</v>
       </c>
       <c r="D121" t="n">
-        <v>26.5</v>
+        <v>23.37</v>
       </c>
       <c r="E121" t="n">
-        <v>11.09</v>
-      </c>
-      <c r="F121" t="n">
-        <v>11.451</v>
-      </c>
-      <c r="G121" t="n">
-        <v>110.262</v>
-      </c>
-      <c r="H121" t="n">
-        <v>10.568</v>
+        <v>19.51</v>
       </c>
     </row>
     <row r="122">
@@ -3454,25 +2757,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>30.53</v>
+        <v>37.57</v>
       </c>
       <c r="C122" t="n">
-        <v>6.67</v>
+        <v>0</v>
       </c>
       <c r="D122" t="n">
-        <v>30.41</v>
+        <v>23.17</v>
       </c>
       <c r="E122" t="n">
-        <v>11.8</v>
-      </c>
-      <c r="F122" t="n">
-        <v>10.017</v>
-      </c>
-      <c r="G122" t="n">
-        <v>111.127</v>
-      </c>
-      <c r="H122" t="n">
-        <v>11.445</v>
+        <v>19.26</v>
       </c>
     </row>
     <row r="123">
@@ -3480,25 +2774,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>29.76</v>
+        <v>37.88</v>
       </c>
       <c r="C123" t="n">
-        <v>6.46</v>
+        <v>0</v>
       </c>
       <c r="D123" t="n">
-        <v>34.8</v>
+        <v>23.19</v>
       </c>
       <c r="E123" t="n">
-        <v>12.36</v>
-      </c>
-      <c r="F123" t="n">
-        <v>8.303000000000001</v>
-      </c>
-      <c r="G123" t="n">
-        <v>112.012</v>
-      </c>
-      <c r="H123" t="n">
-        <v>12.302</v>
+        <v>18.93</v>
       </c>
     </row>
     <row r="124">
@@ -3506,25 +2791,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>29.3</v>
+        <v>37.21</v>
       </c>
       <c r="C124" t="n">
-        <v>6.24</v>
+        <v>0</v>
       </c>
       <c r="D124" t="n">
-        <v>39.21</v>
+        <v>24.18</v>
       </c>
       <c r="E124" t="n">
-        <v>12.45</v>
-      </c>
-      <c r="F124" t="n">
-        <v>6.589</v>
-      </c>
-      <c r="G124" t="n">
-        <v>112.112</v>
-      </c>
-      <c r="H124" t="n">
-        <v>12.106</v>
+        <v>18.61</v>
       </c>
     </row>
     <row r="125">
@@ -3532,25 +2808,16 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>28.74</v>
+        <v>36.38</v>
       </c>
       <c r="C125" t="n">
-        <v>6.04</v>
+        <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>43.63</v>
+        <v>25.15</v>
       </c>
       <c r="E125" t="n">
-        <v>12.83</v>
-      </c>
-      <c r="F125" t="n">
-        <v>4.655</v>
-      </c>
-      <c r="G125" t="n">
-        <v>112.212</v>
-      </c>
-      <c r="H125" t="n">
-        <v>11.89</v>
+        <v>18.47</v>
       </c>
     </row>
     <row r="126">
@@ -3558,25 +2825,16 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>28.2</v>
+        <v>35.25</v>
       </c>
       <c r="C126" t="n">
-        <v>5.82</v>
+        <v>0</v>
       </c>
       <c r="D126" t="n">
-        <v>46.63</v>
+        <v>26.38</v>
       </c>
       <c r="E126" t="n">
-        <v>13.13</v>
-      </c>
-      <c r="F126" t="n">
-        <v>3.54</v>
-      </c>
-      <c r="G126" t="n">
-        <v>112.292</v>
-      </c>
-      <c r="H126" t="n">
-        <v>12.383</v>
+        <v>18.37</v>
       </c>
     </row>
     <row r="127">
@@ -3584,25 +2842,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>27.66</v>
+        <v>34.11</v>
       </c>
       <c r="C127" t="n">
-        <v>5.55</v>
+        <v>0</v>
       </c>
       <c r="D127" t="n">
-        <v>50.93</v>
+        <v>27.6</v>
       </c>
       <c r="E127" t="n">
-        <v>12.04</v>
-      </c>
-      <c r="F127" t="n">
-        <v>2.715</v>
-      </c>
-      <c r="G127" t="n">
-        <v>112.292</v>
-      </c>
-      <c r="H127" t="n">
-        <v>12.816</v>
+        <v>18.29</v>
       </c>
     </row>
     <row r="128">
@@ -3610,25 +2859,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>27.06</v>
+        <v>32.21</v>
       </c>
       <c r="C128" t="n">
-        <v>4.87</v>
+        <v>0</v>
       </c>
       <c r="D128" t="n">
-        <v>55.21</v>
+        <v>29.57</v>
       </c>
       <c r="E128" t="n">
-        <v>10.97</v>
-      </c>
-      <c r="F128" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="G128" t="n">
-        <v>112.292</v>
-      </c>
-      <c r="H128" t="n">
-        <v>13.78</v>
+        <v>18.22</v>
       </c>
     </row>
     <row r="129">
@@ -3636,25 +2876,16 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>26.94</v>
+        <v>30.75</v>
       </c>
       <c r="C129" t="n">
-        <v>4.28</v>
+        <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>57.75</v>
+        <v>31.12</v>
       </c>
       <c r="E129" t="n">
-        <v>10.97</v>
-      </c>
-      <c r="F129" t="n">
-        <v>0.905</v>
-      </c>
-      <c r="G129" t="n">
-        <v>112.292</v>
-      </c>
-      <c r="H129" t="n">
-        <v>14.861</v>
+        <v>18.13</v>
       </c>
     </row>
     <row r="130">
@@ -3662,25 +2893,16 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>26.68</v>
+        <v>29.08</v>
       </c>
       <c r="C130" t="n">
-        <v>3.69</v>
+        <v>0</v>
       </c>
       <c r="D130" t="n">
-        <v>60.25</v>
+        <v>32.62</v>
       </c>
       <c r="E130" t="n">
-        <v>10.97</v>
-      </c>
-      <c r="F130" t="n">
-        <v>0</v>
-      </c>
-      <c r="G130" t="n">
-        <v>112.371</v>
-      </c>
-      <c r="H130" t="n">
-        <v>16.032</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="131">
@@ -3688,25 +2910,16 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>26.49</v>
+        <v>26.98</v>
       </c>
       <c r="C131" t="n">
-        <v>3.1</v>
+        <v>0</v>
       </c>
       <c r="D131" t="n">
-        <v>63.52</v>
+        <v>34.48</v>
       </c>
       <c r="E131" t="n">
-        <v>8.970000000000001</v>
-      </c>
-      <c r="F131" t="n">
-        <v>0</v>
-      </c>
-      <c r="G131" t="n">
-        <v>110.729</v>
-      </c>
-      <c r="H131" t="n">
-        <v>17.2</v>
+        <v>18.54</v>
       </c>
     </row>
     <row r="132">
@@ -3714,25 +2927,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>26.27</v>
+        <v>26.6</v>
       </c>
       <c r="C132" t="n">
-        <v>2.52</v>
+        <v>0</v>
       </c>
       <c r="D132" t="n">
-        <v>66.73</v>
+        <v>34.67</v>
       </c>
       <c r="E132" t="n">
-        <v>6.83</v>
-      </c>
-      <c r="F132" t="n">
-        <v>0</v>
-      </c>
-      <c r="G132" t="n">
-        <v>109.227</v>
-      </c>
-      <c r="H132" t="n">
-        <v>18.418</v>
+        <v>18.73</v>
       </c>
     </row>
     <row r="133">
@@ -3740,25 +2944,16 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>26.06</v>
+        <v>26.25</v>
       </c>
       <c r="C133" t="n">
-        <v>1.97</v>
+        <v>0</v>
       </c>
       <c r="D133" t="n">
-        <v>69.54000000000001</v>
+        <v>34.77</v>
       </c>
       <c r="E133" t="n">
-        <v>5.11</v>
-      </c>
-      <c r="F133" t="n">
-        <v>0</v>
-      </c>
-      <c r="G133" t="n">
-        <v>107.725</v>
-      </c>
-      <c r="H133" t="n">
-        <v>19.586</v>
+        <v>18.99</v>
       </c>
     </row>
     <row r="134">
@@ -3766,25 +2961,16 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>25.69</v>
+        <v>27.77</v>
       </c>
       <c r="C134" t="n">
-        <v>1.44</v>
+        <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>72.34999999999999</v>
+        <v>33.4</v>
       </c>
       <c r="E134" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="F134" t="n">
-        <v>0</v>
-      </c>
-      <c r="G134" t="n">
-        <v>107.314</v>
-      </c>
-      <c r="H134" t="n">
-        <v>19.75</v>
+        <v>19.26</v>
       </c>
     </row>
     <row r="135">
@@ -3792,25 +2978,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>25.71</v>
+        <v>29.36</v>
       </c>
       <c r="C135" t="n">
-        <v>0.92</v>
+        <v>0</v>
       </c>
       <c r="D135" t="n">
-        <v>75.02</v>
+        <v>32.05</v>
       </c>
       <c r="E135" t="n">
-        <v>1.67</v>
-      </c>
-      <c r="F135" t="n">
-        <v>0</v>
-      </c>
-      <c r="G135" t="n">
-        <v>106.893</v>
-      </c>
-      <c r="H135" t="n">
-        <v>19.787</v>
+        <v>19.45</v>
       </c>
     </row>
     <row r="136">
@@ -3818,25 +2995,16 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>25.49</v>
+        <v>31.62</v>
       </c>
       <c r="C136" t="n">
-        <v>0.42</v>
+        <v>0</v>
       </c>
       <c r="D136" t="n">
-        <v>77.41</v>
+        <v>30.69</v>
       </c>
       <c r="E136" t="n">
-        <v>0</v>
-      </c>
-      <c r="F136" t="n">
-        <v>0</v>
-      </c>
-      <c r="G136" t="n">
-        <v>106.492</v>
-      </c>
-      <c r="H136" t="n">
-        <v>20.187</v>
+        <v>18.98</v>
       </c>
     </row>
     <row r="137">
@@ -3844,25 +3012,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>25.25</v>
+        <v>33.97</v>
       </c>
       <c r="C137" t="n">
         <v>0</v>
       </c>
       <c r="D137" t="n">
-        <v>77.87</v>
+        <v>29.39</v>
       </c>
       <c r="E137" t="n">
-        <v>0</v>
-      </c>
-      <c r="F137" t="n">
-        <v>0</v>
-      </c>
-      <c r="G137" t="n">
-        <v>106.171</v>
-      </c>
-      <c r="H137" t="n">
-        <v>20.707</v>
+        <v>18.35</v>
       </c>
     </row>
     <row r="138">
@@ -3870,25 +3029,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>25.05</v>
+        <v>36.79</v>
       </c>
       <c r="C138" t="n">
         <v>0</v>
       </c>
       <c r="D138" t="n">
-        <v>78.38</v>
+        <v>27.22</v>
       </c>
       <c r="E138" t="n">
-        <v>0</v>
-      </c>
-      <c r="F138" t="n">
-        <v>0</v>
-      </c>
-      <c r="G138" t="n">
-        <v>105.87</v>
-      </c>
-      <c r="H138" t="n">
-        <v>20.696</v>
+        <v>17.71</v>
       </c>
     </row>
     <row r="139">
@@ -3896,25 +3046,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>24.5</v>
+        <v>39.37</v>
       </c>
       <c r="C139" t="n">
         <v>0</v>
       </c>
       <c r="D139" t="n">
-        <v>78.84999999999999</v>
+        <v>25.28</v>
       </c>
       <c r="E139" t="n">
-        <v>0</v>
-      </c>
-      <c r="F139" t="n">
-        <v>0</v>
-      </c>
-      <c r="G139" t="n">
-        <v>106.048</v>
-      </c>
-      <c r="H139" t="n">
-        <v>20.598</v>
+        <v>17.07</v>
       </c>
     </row>
     <row r="140">
@@ -3922,25 +3063,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>24.04</v>
+        <v>42.07</v>
       </c>
       <c r="C140" t="n">
         <v>0</v>
       </c>
       <c r="D140" t="n">
-        <v>79.3</v>
+        <v>23.26</v>
       </c>
       <c r="E140" t="n">
-        <v>0</v>
-      </c>
-      <c r="F140" t="n">
-        <v>0</v>
-      </c>
-      <c r="G140" t="n">
-        <v>106.266</v>
-      </c>
-      <c r="H140" t="n">
-        <v>20.4</v>
+        <v>16.39</v>
       </c>
     </row>
     <row r="141">
@@ -3948,25 +3080,19 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>23.56</v>
+        <v>44.39</v>
       </c>
       <c r="C141" t="n">
         <v>0</v>
       </c>
       <c r="D141" t="n">
-        <v>79.02</v>
+        <v>21.62</v>
       </c>
       <c r="E141" t="n">
-        <v>0</v>
+        <v>15.71</v>
       </c>
       <c r="F141" t="n">
-        <v>0</v>
-      </c>
-      <c r="G141" t="n">
-        <v>107.129</v>
-      </c>
-      <c r="H141" t="n">
-        <v>20.292</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142">
@@ -3974,25 +3100,19 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>23.1</v>
+        <v>44.81</v>
       </c>
       <c r="C142" t="n">
         <v>0</v>
       </c>
       <c r="D142" t="n">
-        <v>79.34</v>
+        <v>22.58</v>
       </c>
       <c r="E142" t="n">
-        <v>0</v>
+        <v>14.33</v>
       </c>
       <c r="F142" t="n">
-        <v>0</v>
-      </c>
-      <c r="G142" t="n">
-        <v>107.368</v>
-      </c>
-      <c r="H142" t="n">
-        <v>20.187</v>
+        <v>19.715</v>
       </c>
     </row>
     <row r="143">
@@ -4000,25 +3120,19 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>22.08</v>
+        <v>45.23</v>
       </c>
       <c r="C143" t="n">
         <v>0</v>
       </c>
       <c r="D143" t="n">
-        <v>79.54000000000001</v>
+        <v>23.41</v>
       </c>
       <c r="E143" t="n">
-        <v>0</v>
+        <v>13.13</v>
       </c>
       <c r="F143" t="n">
-        <v>0</v>
-      </c>
-      <c r="G143" t="n">
-        <v>107.562</v>
-      </c>
-      <c r="H143" t="n">
-        <v>20.82200000000001</v>
+        <v>19.55333333333333</v>
       </c>
     </row>
     <row r="144">
@@ -4026,25 +3140,19 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>21.39</v>
+        <v>45.27</v>
       </c>
       <c r="C144" t="n">
         <v>0</v>
       </c>
       <c r="D144" t="n">
-        <v>79.73</v>
+        <v>24.23</v>
       </c>
       <c r="E144" t="n">
-        <v>0</v>
+        <v>11.93</v>
       </c>
       <c r="F144" t="n">
-        <v>0</v>
-      </c>
-      <c r="G144" t="n">
-        <v>107.522</v>
-      </c>
-      <c r="H144" t="n">
-        <v>21.364</v>
+        <v>19.4475</v>
       </c>
     </row>
     <row r="145">
@@ -4052,25 +3160,19 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>20.41</v>
+        <v>45.48</v>
       </c>
       <c r="C145" t="n">
         <v>0</v>
       </c>
       <c r="D145" t="n">
-        <v>80.06</v>
+        <v>24.79</v>
       </c>
       <c r="E145" t="n">
-        <v>0</v>
+        <v>10.81</v>
       </c>
       <c r="F145" t="n">
-        <v>0</v>
-      </c>
-      <c r="G145" t="n">
-        <v>107.492</v>
-      </c>
-      <c r="H145" t="n">
-        <v>22.033</v>
+        <v>19.384</v>
       </c>
     </row>
     <row r="146">
@@ -4078,25 +3180,19 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>19.68</v>
+        <v>45.01</v>
       </c>
       <c r="C146" t="n">
         <v>0</v>
       </c>
       <c r="D146" t="n">
-        <v>80.58</v>
+        <v>25.31</v>
       </c>
       <c r="E146" t="n">
-        <v>0</v>
+        <v>10.41</v>
       </c>
       <c r="F146" t="n">
-        <v>0</v>
-      </c>
-      <c r="G146" t="n">
-        <v>107.442</v>
-      </c>
-      <c r="H146" t="n">
-        <v>22.289</v>
+        <v>18.96166666666667</v>
       </c>
     </row>
     <row r="147">
@@ -4104,25 +3200,19 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>18.85</v>
+        <v>44.47</v>
       </c>
       <c r="C147" t="n">
         <v>0</v>
       </c>
       <c r="D147" t="n">
-        <v>80.73999999999999</v>
+        <v>25.78</v>
       </c>
       <c r="E147" t="n">
-        <v>0</v>
+        <v>10.38</v>
       </c>
       <c r="F147" t="n">
-        <v>0</v>
-      </c>
-      <c r="G147" t="n">
-        <v>107.382</v>
-      </c>
-      <c r="H147" t="n">
-        <v>23.034</v>
+        <v>18.53142857142857</v>
       </c>
     </row>
     <row r="148">
@@ -4130,25 +3220,19 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>17.99</v>
+        <v>43.9</v>
       </c>
       <c r="C148" t="n">
         <v>0</v>
       </c>
       <c r="D148" t="n">
-        <v>80.81999999999999</v>
+        <v>26.77</v>
       </c>
       <c r="E148" t="n">
-        <v>0</v>
+        <v>10.35</v>
       </c>
       <c r="F148" t="n">
-        <v>0</v>
-      </c>
-      <c r="G148" t="n">
-        <v>107.302</v>
-      </c>
-      <c r="H148" t="n">
-        <v>23.889</v>
+        <v>18.23375</v>
       </c>
     </row>
     <row r="149">
@@ -4156,25 +3240,19 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>17.49</v>
+        <v>43.34</v>
       </c>
       <c r="C149" t="n">
         <v>0</v>
       </c>
       <c r="D149" t="n">
-        <v>81.61</v>
+        <v>27.73</v>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>10.34</v>
       </c>
       <c r="F149" t="n">
-        <v>0</v>
-      </c>
-      <c r="G149" t="n">
-        <v>106.743</v>
-      </c>
-      <c r="H149" t="n">
-        <v>24.161</v>
+        <v>17.93555555555555</v>
       </c>
     </row>
     <row r="150">
@@ -4182,25 +3260,19 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>16.81</v>
+        <v>42.8</v>
       </c>
       <c r="C150" t="n">
         <v>0</v>
       </c>
       <c r="D150" t="n">
-        <v>82.39</v>
+        <v>28.91</v>
       </c>
       <c r="E150" t="n">
-        <v>0</v>
+        <v>10.16</v>
       </c>
       <c r="F150" t="n">
-        <v>0</v>
-      </c>
-      <c r="G150" t="n">
-        <v>106.44</v>
-      </c>
-      <c r="H150" t="n">
-        <v>24.361</v>
+        <v>16.512</v>
       </c>
     </row>
     <row r="151">
@@ -4208,25 +3280,19 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>16.08</v>
+        <v>42.68</v>
       </c>
       <c r="C151" t="n">
         <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>83.13</v>
+        <v>29.6</v>
       </c>
       <c r="E151" t="n">
-        <v>0</v>
+        <v>11.21</v>
       </c>
       <c r="F151" t="n">
-        <v>0</v>
-      </c>
-      <c r="G151" t="n">
-        <v>106.308</v>
-      </c>
-      <c r="H151" t="n">
-        <v>24.474</v>
+        <v>16.512</v>
       </c>
     </row>
     <row r="152">
@@ -4234,25 +3300,19 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>15.34</v>
+        <v>42.85</v>
       </c>
       <c r="C152" t="n">
         <v>0</v>
       </c>
       <c r="D152" t="n">
-        <v>83.33</v>
+        <v>29.34</v>
       </c>
       <c r="E152" t="n">
-        <v>0</v>
+        <v>12.99</v>
       </c>
       <c r="F152" t="n">
-        <v>0</v>
-      </c>
-      <c r="G152" t="n">
-        <v>106.77</v>
-      </c>
-      <c r="H152" t="n">
-        <v>24.564</v>
+        <v>14.822</v>
       </c>
     </row>
     <row r="153">
@@ -4260,25 +3320,19 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>15.06</v>
+        <v>43.98</v>
       </c>
       <c r="C153" t="n">
         <v>0</v>
       </c>
       <c r="D153" t="n">
-        <v>83.7</v>
+        <v>28.31</v>
       </c>
       <c r="E153" t="n">
-        <v>0</v>
+        <v>14.53</v>
       </c>
       <c r="F153" t="n">
-        <v>0</v>
-      </c>
-      <c r="G153" t="n">
-        <v>107.277</v>
-      </c>
-      <c r="H153" t="n">
-        <v>23.96400000000001</v>
+        <v>13.179</v>
       </c>
     </row>
     <row r="154">
@@ -4286,25 +3340,19 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>14.74</v>
+        <v>45.21</v>
       </c>
       <c r="C154" t="n">
         <v>0</v>
       </c>
       <c r="D154" t="n">
-        <v>84.08</v>
+        <v>27.24</v>
       </c>
       <c r="E154" t="n">
-        <v>0</v>
+        <v>15.99</v>
       </c>
       <c r="F154" t="n">
-        <v>0</v>
-      </c>
-      <c r="G154" t="n">
-        <v>107.727</v>
-      </c>
-      <c r="H154" t="n">
-        <v>23.457</v>
+        <v>11.556</v>
       </c>
     </row>
     <row r="155">
@@ -4312,25 +3360,19 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>14.48</v>
+        <v>45.84</v>
       </c>
       <c r="C155" t="n">
         <v>0</v>
       </c>
       <c r="D155" t="n">
-        <v>84.43000000000001</v>
+        <v>26.41</v>
       </c>
       <c r="E155" t="n">
-        <v>0</v>
+        <v>17.81</v>
       </c>
       <c r="F155" t="n">
-        <v>0</v>
-      </c>
-      <c r="G155" t="n">
-        <v>108.167</v>
-      </c>
-      <c r="H155" t="n">
-        <v>22.913</v>
+        <v>9.943000000000001</v>
       </c>
     </row>
     <row r="156">
@@ -4338,25 +3380,679 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>14.18</v>
+        <v>46.5</v>
       </c>
       <c r="C156" t="n">
         <v>0</v>
       </c>
       <c r="D156" t="n">
-        <v>84.86</v>
+        <v>25.61</v>
       </c>
       <c r="E156" t="n">
-        <v>0</v>
+        <v>19.58</v>
       </c>
       <c r="F156" t="n">
-        <v>0</v>
-      </c>
-      <c r="G156" t="n">
-        <v>108.627</v>
-      </c>
-      <c r="H156" t="n">
-        <v>22.329</v>
+        <v>8.309999999999999</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0</v>
+      </c>
+      <c r="D157" t="n">
+        <v>24.79</v>
+      </c>
+      <c r="E157" t="n">
+        <v>21.01</v>
+      </c>
+      <c r="F157" t="n">
+        <v>6.895</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="n">
+        <v>48.11</v>
+      </c>
+      <c r="C158" t="n">
+        <v>0</v>
+      </c>
+      <c r="D158" t="n">
+        <v>23.95</v>
+      </c>
+      <c r="E158" t="n">
+        <v>22.43</v>
+      </c>
+      <c r="F158" t="n">
+        <v>5.513</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="n">
+        <v>49.02</v>
+      </c>
+      <c r="C159" t="n">
+        <v>0</v>
+      </c>
+      <c r="D159" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="E159" t="n">
+        <v>23.83</v>
+      </c>
+      <c r="F159" t="n">
+        <v>4.111</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="n">
+        <v>50.08</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0</v>
+      </c>
+      <c r="D160" t="n">
+        <v>20.05</v>
+      </c>
+      <c r="E160" t="n">
+        <v>25.17</v>
+      </c>
+      <c r="F160" t="n">
+        <v>2.749</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="n">
+        <v>51.2</v>
+      </c>
+      <c r="C161" t="n">
+        <v>0</v>
+      </c>
+      <c r="D161" t="n">
+        <v>18.99</v>
+      </c>
+      <c r="E161" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="F161" t="n">
+        <v>4.561999999999999</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="n">
+        <v>52.69</v>
+      </c>
+      <c r="C162" t="n">
+        <v>0</v>
+      </c>
+      <c r="D162" t="n">
+        <v>17.97</v>
+      </c>
+      <c r="E162" t="n">
+        <v>25.42</v>
+      </c>
+      <c r="F162" t="n">
+        <v>5.976</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="n">
+        <v>53.27</v>
+      </c>
+      <c r="C163" t="n">
+        <v>0</v>
+      </c>
+      <c r="D163" t="n">
+        <v>17.67</v>
+      </c>
+      <c r="E163" t="n">
+        <v>25.72</v>
+      </c>
+      <c r="F163" t="n">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="C164" t="n">
+        <v>0</v>
+      </c>
+      <c r="D164" t="n">
+        <v>17.45</v>
+      </c>
+      <c r="E164" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="F164" t="n">
+        <v>8.803999999999998</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="n">
+        <v>54.97</v>
+      </c>
+      <c r="C165" t="n">
+        <v>0</v>
+      </c>
+      <c r="D165" t="n">
+        <v>16.78</v>
+      </c>
+      <c r="E165" t="n">
+        <v>26.11</v>
+      </c>
+      <c r="F165" t="n">
+        <v>10.198</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="n">
+        <v>56.22</v>
+      </c>
+      <c r="C166" t="n">
+        <v>0</v>
+      </c>
+      <c r="D166" t="n">
+        <v>16.09</v>
+      </c>
+      <c r="E166" t="n">
+        <v>26.16</v>
+      </c>
+      <c r="F166" t="n">
+        <v>11.592</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="n">
+        <v>57.29</v>
+      </c>
+      <c r="C167" t="n">
+        <v>0</v>
+      </c>
+      <c r="D167" t="n">
+        <v>15.63</v>
+      </c>
+      <c r="E167" t="n">
+        <v>26.13</v>
+      </c>
+      <c r="F167" t="n">
+        <v>12.996</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="n">
+        <v>58.36</v>
+      </c>
+      <c r="C168" t="n">
+        <v>0</v>
+      </c>
+      <c r="D168" t="n">
+        <v>15.18</v>
+      </c>
+      <c r="E168" t="n">
+        <v>26.12</v>
+      </c>
+      <c r="F168" t="n">
+        <v>14.387</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="n">
+        <v>59.34</v>
+      </c>
+      <c r="C169" t="n">
+        <v>0</v>
+      </c>
+      <c r="D169" t="n">
+        <v>16.84</v>
+      </c>
+      <c r="E169" t="n">
+        <v>26.12</v>
+      </c>
+      <c r="F169" t="n">
+        <v>15.768</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="n">
+        <v>60.3</v>
+      </c>
+      <c r="C170" t="n">
+        <v>0</v>
+      </c>
+      <c r="D170" t="n">
+        <v>16.47</v>
+      </c>
+      <c r="E170" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="F170" t="n">
+        <v>17.169</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="n">
+        <v>61.2</v>
+      </c>
+      <c r="C171" t="n">
+        <v>0</v>
+      </c>
+      <c r="D171" t="n">
+        <v>16.18</v>
+      </c>
+      <c r="E171" t="n">
+        <v>26.25</v>
+      </c>
+      <c r="F171" t="n">
+        <v>16.58</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="n">
+        <v>62.23</v>
+      </c>
+      <c r="C172" t="n">
+        <v>0</v>
+      </c>
+      <c r="D172" t="n">
+        <v>15.31</v>
+      </c>
+      <c r="E172" t="n">
+        <v>26.31</v>
+      </c>
+      <c r="F172" t="n">
+        <v>16.43</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="n">
+        <v>63.06</v>
+      </c>
+      <c r="C173" t="n">
+        <v>0</v>
+      </c>
+      <c r="D173" t="n">
+        <v>14.54</v>
+      </c>
+      <c r="E173" t="n">
+        <v>26.25</v>
+      </c>
+      <c r="F173" t="n">
+        <v>16.52</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="n">
+        <v>63.92</v>
+      </c>
+      <c r="C174" t="n">
+        <v>0</v>
+      </c>
+      <c r="D174" t="n">
+        <v>13.72</v>
+      </c>
+      <c r="E174" t="n">
+        <v>26.19</v>
+      </c>
+      <c r="F174" t="n">
+        <v>16.61</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="n">
+        <v>64.27</v>
+      </c>
+      <c r="C175" t="n">
+        <v>0</v>
+      </c>
+      <c r="D175" t="n">
+        <v>13.31</v>
+      </c>
+      <c r="E175" t="n">
+        <v>26.15</v>
+      </c>
+      <c r="F175" t="n">
+        <v>16.777</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="n">
+        <v>64.72</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0</v>
+      </c>
+      <c r="D176" t="n">
+        <v>12.85</v>
+      </c>
+      <c r="E176" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F176" t="n">
+        <v>16.944</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="n">
+        <v>65.38</v>
+      </c>
+      <c r="C177" t="n">
+        <v>0</v>
+      </c>
+      <c r="D177" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="E177" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F177" t="n">
+        <v>17.046</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="n">
+        <v>66.28</v>
+      </c>
+      <c r="C178" t="n">
+        <v>0</v>
+      </c>
+      <c r="D178" t="n">
+        <v>11.36</v>
+      </c>
+      <c r="E178" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F178" t="n">
+        <v>17.003</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="n">
+        <v>67.17</v>
+      </c>
+      <c r="C179" t="n">
+        <v>0</v>
+      </c>
+      <c r="D179" t="n">
+        <v>10.55</v>
+      </c>
+      <c r="E179" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F179" t="n">
+        <v>16.925</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="n">
+        <v>68.15000000000001</v>
+      </c>
+      <c r="C180" t="n">
+        <v>0</v>
+      </c>
+      <c r="D180" t="n">
+        <v>9.68</v>
+      </c>
+      <c r="E180" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F180" t="n">
+        <v>16.827</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="n">
+        <v>69.18000000000001</v>
+      </c>
+      <c r="C181" t="n">
+        <v>0</v>
+      </c>
+      <c r="D181" t="n">
+        <v>8.76</v>
+      </c>
+      <c r="E181" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F181" t="n">
+        <v>16.709</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="n">
+        <v>69.53</v>
+      </c>
+      <c r="C182" t="n">
+        <v>0</v>
+      </c>
+      <c r="D182" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="E182" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F182" t="n">
+        <v>16.611</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="n">
+        <v>70.33</v>
+      </c>
+      <c r="C183" t="n">
+        <v>0</v>
+      </c>
+      <c r="D183" t="n">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="E183" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F183" t="n">
+        <v>16.253</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="n">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="C184" t="n">
+        <v>0</v>
+      </c>
+      <c r="D184" t="n">
+        <v>7.49</v>
+      </c>
+      <c r="E184" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F184" t="n">
+        <v>16.035</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="n">
+        <v>72.36</v>
+      </c>
+      <c r="C185" t="n">
+        <v>0</v>
+      </c>
+      <c r="D185" t="n">
+        <v>6.54</v>
+      </c>
+      <c r="E185" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F185" t="n">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="n">
+        <v>74.84999999999999</v>
+      </c>
+      <c r="C186" t="n">
+        <v>0</v>
+      </c>
+      <c r="D186" t="n">
+        <v>5.67</v>
+      </c>
+      <c r="E186" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F186" t="n">
+        <v>14.105</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="n">
+        <v>77.23</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0</v>
+      </c>
+      <c r="D187" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="E187" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F187" t="n">
+        <v>12.535</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="n">
+        <v>79.37</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0</v>
+      </c>
+      <c r="D188" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="E188" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F188" t="n">
+        <v>11.18</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="n">
+        <v>81.54000000000001</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0</v>
+      </c>
+      <c r="D189" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="E189" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F189" t="n">
+        <v>9.860000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added hands played to command line output
</commit_message>
<xml_diff>
--- a/Outputs/stacks_over_time_avg.xlsx
+++ b/Outputs/stacks_over_time_avg.xlsx
@@ -194,7 +194,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$B$2:$B$227</f>
+              <f>'data'!$B$2:$B$189</f>
             </numRef>
           </val>
         </ser>
@@ -221,7 +221,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$C$2:$C$227</f>
+              <f>'data'!$C$2:$C$189</f>
             </numRef>
           </val>
         </ser>
@@ -248,7 +248,61 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$D$2:$D$227</f>
+              <f>'data'!$D$2:$D$189</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <strRef>
+              <f>'data'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'data'!$E$2:$E$189</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <strRef>
+              <f>'data'!F1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'data'!$F$2:$F$189</f>
             </numRef>
           </val>
         </ser>
@@ -618,7 +672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D227"/>
+  <dimension ref="A1:F189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -634,12 +688,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Raymond</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cedric</t>
+          <t>Ben</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -647,6 +701,16 @@
           <t>Fish</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cedric</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Raymond</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -659,6 +723,9 @@
         <v>20</v>
       </c>
       <c r="D2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2" t="n">
         <v>20</v>
       </c>
     </row>
@@ -667,13 +734,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20.38</v>
+        <v>20.5</v>
       </c>
       <c r="C3" t="n">
-        <v>19.71</v>
+        <v>19.5</v>
       </c>
       <c r="D3" t="n">
-        <v>19.9</v>
+        <v>20</v>
+      </c>
+      <c r="E3" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -681,13 +751,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20.21</v>
+        <v>20.67</v>
       </c>
       <c r="C4" t="n">
-        <v>19.55</v>
+        <v>19.33</v>
       </c>
       <c r="D4" t="n">
-        <v>20.23</v>
+        <v>20</v>
+      </c>
+      <c r="E4" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -695,13 +768,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20.18</v>
+        <v>21.2</v>
       </c>
       <c r="C5" t="n">
-        <v>19.42</v>
+        <v>19.05</v>
       </c>
       <c r="D5" t="n">
-        <v>20.4</v>
+        <v>19.8</v>
+      </c>
+      <c r="E5" t="n">
+        <v>19.95</v>
       </c>
     </row>
     <row r="6">
@@ -709,13 +785,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20.16</v>
+        <v>21.44</v>
       </c>
       <c r="C6" t="n">
-        <v>19.32</v>
+        <v>18.84</v>
       </c>
       <c r="D6" t="n">
-        <v>20.52</v>
+        <v>19.68</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20.04</v>
       </c>
     </row>
     <row r="7">
@@ -723,13 +802,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20.19</v>
+        <v>21.15</v>
       </c>
       <c r="C7" t="n">
-        <v>19.22</v>
+        <v>17.92</v>
       </c>
       <c r="D7" t="n">
-        <v>20.58</v>
+        <v>20.83</v>
+      </c>
+      <c r="E7" t="n">
+        <v>20.1</v>
       </c>
     </row>
     <row r="8">
@@ -737,13 +819,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20.12</v>
+        <v>20.94</v>
       </c>
       <c r="C8" t="n">
-        <v>19.34</v>
+        <v>17.2</v>
       </c>
       <c r="D8" t="n">
-        <v>20.54</v>
+        <v>21.71</v>
+      </c>
+      <c r="E8" t="n">
+        <v>20.14</v>
       </c>
     </row>
     <row r="9">
@@ -751,13 +836,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20.07</v>
+        <v>21.01</v>
       </c>
       <c r="C9" t="n">
-        <v>19.35</v>
+        <v>16.56</v>
       </c>
       <c r="D9" t="n">
-        <v>20.58</v>
+        <v>22.28</v>
+      </c>
+      <c r="E9" t="n">
+        <v>20.15</v>
       </c>
     </row>
     <row r="10">
@@ -765,13 +853,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>19.99</v>
+        <v>20.88</v>
       </c>
       <c r="C10" t="n">
-        <v>19.36</v>
+        <v>16.29</v>
       </c>
       <c r="D10" t="n">
-        <v>20.65</v>
+        <v>22.69</v>
+      </c>
+      <c r="E10" t="n">
+        <v>20.14</v>
       </c>
     </row>
     <row r="11">
@@ -779,13 +870,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19.9</v>
+        <v>21.06</v>
       </c>
       <c r="C11" t="n">
-        <v>19.41</v>
+        <v>16.05</v>
       </c>
       <c r="D11" t="n">
-        <v>20.69</v>
+        <v>23</v>
+      </c>
+      <c r="E11" t="n">
+        <v>19.89</v>
       </c>
     </row>
     <row r="12">
@@ -793,13 +887,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>19.9</v>
+        <v>21.06</v>
       </c>
       <c r="C12" t="n">
-        <v>19.41</v>
+        <v>16.05</v>
       </c>
       <c r="D12" t="n">
-        <v>20.69</v>
+        <v>23</v>
+      </c>
+      <c r="E12" t="n">
+        <v>19.89</v>
       </c>
     </row>
     <row r="13">
@@ -807,13 +904,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19.82</v>
+        <v>21.32</v>
       </c>
       <c r="C13" t="n">
-        <v>19.41</v>
+        <v>15.47</v>
       </c>
       <c r="D13" t="n">
-        <v>20.78</v>
+        <v>23.56</v>
+      </c>
+      <c r="E13" t="n">
+        <v>19.65</v>
       </c>
     </row>
     <row r="14">
@@ -821,13 +921,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19.67</v>
+        <v>21.23</v>
       </c>
       <c r="C14" t="n">
-        <v>19.47</v>
+        <v>14.92</v>
       </c>
       <c r="D14" t="n">
-        <v>20.86</v>
+        <v>24.46</v>
+      </c>
+      <c r="E14" t="n">
+        <v>19.39</v>
       </c>
     </row>
     <row r="15">
@@ -835,13 +938,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>19.59</v>
+        <v>21.2</v>
       </c>
       <c r="C15" t="n">
-        <v>19.83</v>
+        <v>14.37</v>
       </c>
       <c r="D15" t="n">
-        <v>20.58</v>
+        <v>25.31</v>
+      </c>
+      <c r="E15" t="n">
+        <v>19.12</v>
       </c>
     </row>
     <row r="16">
@@ -849,13 +955,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>19.57</v>
+        <v>21.14</v>
       </c>
       <c r="C16" t="n">
-        <v>20.2</v>
+        <v>13.88</v>
       </c>
       <c r="D16" t="n">
-        <v>20.23</v>
+        <v>26.11</v>
+      </c>
+      <c r="E16" t="n">
+        <v>18.87</v>
       </c>
     </row>
     <row r="17">
@@ -863,13 +972,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>19.56</v>
+        <v>21.12</v>
       </c>
       <c r="C17" t="n">
-        <v>20.58</v>
+        <v>13.43</v>
       </c>
       <c r="D17" t="n">
-        <v>19.86</v>
+        <v>26.91</v>
+      </c>
+      <c r="E17" t="n">
+        <v>18.56</v>
       </c>
     </row>
     <row r="18">
@@ -877,13 +989,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>19.37</v>
+        <v>22.27</v>
       </c>
       <c r="C18" t="n">
-        <v>21.13</v>
+        <v>12.58</v>
       </c>
       <c r="D18" t="n">
-        <v>19.5</v>
+        <v>26.96</v>
+      </c>
+      <c r="E18" t="n">
+        <v>18.23</v>
       </c>
     </row>
     <row r="19">
@@ -891,13 +1006,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>19.25</v>
+        <v>23.37</v>
       </c>
       <c r="C19" t="n">
-        <v>21.5</v>
+        <v>11.7</v>
       </c>
       <c r="D19" t="n">
-        <v>19.25</v>
+        <v>26.96</v>
+      </c>
+      <c r="E19" t="n">
+        <v>18.02</v>
       </c>
     </row>
     <row r="20">
@@ -905,13 +1023,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>19.13</v>
+        <v>24.43</v>
       </c>
       <c r="C20" t="n">
-        <v>21.93</v>
+        <v>10.78</v>
       </c>
       <c r="D20" t="n">
-        <v>18.94</v>
+        <v>27</v>
+      </c>
+      <c r="E20" t="n">
+        <v>17.83</v>
       </c>
     </row>
     <row r="21">
@@ -919,13 +1040,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>19.11</v>
+        <v>26.44</v>
       </c>
       <c r="C21" t="n">
-        <v>22.31</v>
+        <v>9.65</v>
       </c>
       <c r="D21" t="n">
-        <v>18.58</v>
+        <v>26.3</v>
+      </c>
+      <c r="E21" t="n">
+        <v>17.65</v>
       </c>
     </row>
     <row r="22">
@@ -933,13 +1057,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>19.18</v>
+        <v>28.16</v>
       </c>
       <c r="C22" t="n">
-        <v>22.64</v>
+        <v>8.52</v>
       </c>
       <c r="D22" t="n">
-        <v>18.18</v>
+        <v>25.61</v>
+      </c>
+      <c r="E22" t="n">
+        <v>17.76</v>
       </c>
     </row>
     <row r="23">
@@ -947,13 +1074,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>19.22</v>
+        <v>29.61</v>
       </c>
       <c r="C23" t="n">
-        <v>22.99</v>
+        <v>7.71</v>
       </c>
       <c r="D23" t="n">
-        <v>17.79</v>
+        <v>24.87</v>
+      </c>
+      <c r="E23" t="n">
+        <v>17.86</v>
       </c>
     </row>
     <row r="24">
@@ -961,13 +1091,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>19.28</v>
+        <v>32.01</v>
       </c>
       <c r="C24" t="n">
-        <v>23.32</v>
+        <v>6.35</v>
       </c>
       <c r="D24" t="n">
-        <v>17.4</v>
+        <v>23.7</v>
+      </c>
+      <c r="E24" t="n">
+        <v>17.98</v>
       </c>
     </row>
     <row r="25">
@@ -975,13 +1108,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>19.37</v>
+        <v>34.37</v>
       </c>
       <c r="C25" t="n">
-        <v>23.39</v>
+        <v>5</v>
       </c>
       <c r="D25" t="n">
-        <v>17.24</v>
+        <v>22.56</v>
+      </c>
+      <c r="E25" t="n">
+        <v>18.11</v>
       </c>
     </row>
     <row r="26">
@@ -989,13 +1125,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>19.43</v>
+        <v>36.6</v>
       </c>
       <c r="C26" t="n">
-        <v>23.45</v>
+        <v>3.67</v>
       </c>
       <c r="D26" t="n">
-        <v>17.12</v>
+        <v>21.55</v>
+      </c>
+      <c r="E26" t="n">
+        <v>18.22</v>
       </c>
     </row>
     <row r="27">
@@ -1003,13 +1142,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>19.45</v>
+        <v>38.81</v>
       </c>
       <c r="C27" t="n">
-        <v>23.54</v>
+        <v>2.32</v>
       </c>
       <c r="D27" t="n">
-        <v>17.01</v>
+        <v>20.57</v>
+      </c>
+      <c r="E27" t="n">
+        <v>18.32</v>
       </c>
     </row>
     <row r="28">
@@ -1017,13 +1159,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>19.63</v>
+        <v>39.82</v>
       </c>
       <c r="C28" t="n">
-        <v>23.47</v>
+        <v>1.85</v>
       </c>
       <c r="D28" t="n">
-        <v>16.9</v>
+        <v>19.89</v>
+      </c>
+      <c r="E28" t="n">
+        <v>18.44</v>
       </c>
     </row>
     <row r="29">
@@ -1031,13 +1176,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>19.75</v>
+        <v>40.9</v>
       </c>
       <c r="C29" t="n">
-        <v>23.45</v>
+        <v>1.44</v>
       </c>
       <c r="D29" t="n">
-        <v>16.8</v>
+        <v>19.22</v>
+      </c>
+      <c r="E29" t="n">
+        <v>18.45</v>
       </c>
     </row>
     <row r="30">
@@ -1045,13 +1193,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>19.77</v>
+        <v>41.83</v>
       </c>
       <c r="C30" t="n">
-        <v>23.22</v>
+        <v>1.14</v>
       </c>
       <c r="D30" t="n">
-        <v>17.01</v>
+        <v>18.58</v>
+      </c>
+      <c r="E30" t="n">
+        <v>18.45</v>
       </c>
     </row>
     <row r="31">
@@ -1059,13 +1210,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>19.77</v>
+        <v>42.03</v>
       </c>
       <c r="C31" t="n">
-        <v>23.03</v>
+        <v>0.86</v>
       </c>
       <c r="D31" t="n">
-        <v>17.2</v>
+        <v>18.68</v>
+      </c>
+      <c r="E31" t="n">
+        <v>18.43</v>
       </c>
     </row>
     <row r="32">
@@ -1073,13 +1227,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>19.76</v>
+        <v>42.23</v>
       </c>
       <c r="C32" t="n">
-        <v>22.84</v>
+        <v>0.6</v>
       </c>
       <c r="D32" t="n">
-        <v>17.4</v>
+        <v>18.48</v>
+      </c>
+      <c r="E32" t="n">
+        <v>18.69</v>
       </c>
     </row>
     <row r="33">
@@ -1087,13 +1244,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>19.74</v>
+        <v>42.05</v>
       </c>
       <c r="C33" t="n">
-        <v>22.72</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>17.54</v>
+        <v>18.35</v>
+      </c>
+      <c r="E33" t="n">
+        <v>19.6</v>
       </c>
     </row>
     <row r="34">
@@ -1101,13 +1261,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>19.68</v>
+        <v>41.21</v>
       </c>
       <c r="C34" t="n">
-        <v>22.61</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>17.71</v>
+        <v>18.28</v>
+      </c>
+      <c r="E34" t="n">
+        <v>20.51</v>
       </c>
     </row>
     <row r="35">
@@ -1115,13 +1278,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>19.59</v>
+        <v>40.35</v>
       </c>
       <c r="C35" t="n">
-        <v>22.56</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>17.85</v>
+        <v>18.21</v>
+      </c>
+      <c r="E35" t="n">
+        <v>21.44</v>
       </c>
     </row>
     <row r="36">
@@ -1129,13 +1295,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>19.44</v>
+        <v>39.47</v>
       </c>
       <c r="C36" t="n">
-        <v>22.56</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>18</v>
+        <v>18.15</v>
+      </c>
+      <c r="E36" t="n">
+        <v>22.38</v>
       </c>
     </row>
     <row r="37">
@@ -1143,13 +1312,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>19.31</v>
+        <v>38.69</v>
       </c>
       <c r="C37" t="n">
-        <v>22.54</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>18.15</v>
+        <v>17.98</v>
+      </c>
+      <c r="E37" t="n">
+        <v>23.33</v>
       </c>
     </row>
     <row r="38">
@@ -1157,13 +1329,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>18.58</v>
+        <v>38.21</v>
       </c>
       <c r="C38" t="n">
-        <v>22.54</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>18.88</v>
+        <v>17.55</v>
+      </c>
+      <c r="E38" t="n">
+        <v>24.24</v>
       </c>
     </row>
     <row r="39">
@@ -1171,13 +1346,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>17.94</v>
+        <v>37.65</v>
       </c>
       <c r="C39" t="n">
-        <v>22.52</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>19.54</v>
+        <v>17.22</v>
+      </c>
+      <c r="E39" t="n">
+        <v>25.13</v>
       </c>
     </row>
     <row r="40">
@@ -1185,13 +1363,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>17.39</v>
+        <v>36.82</v>
       </c>
       <c r="C40" t="n">
-        <v>22.7</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>19.91</v>
+        <v>16.87</v>
+      </c>
+      <c r="E40" t="n">
+        <v>26.31</v>
       </c>
     </row>
     <row r="41">
@@ -1199,13 +1380,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>16.79</v>
+        <v>35.94</v>
       </c>
       <c r="C41" t="n">
-        <v>22.89</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>20.32</v>
+        <v>16.52</v>
+      </c>
+      <c r="E41" t="n">
+        <v>27.54</v>
       </c>
     </row>
     <row r="42">
@@ -1213,13 +1397,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>17.12</v>
+        <v>34.99</v>
       </c>
       <c r="C42" t="n">
-        <v>23.06</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>20.82</v>
+        <v>16.57</v>
+      </c>
+      <c r="E42" t="n">
+        <v>28.44</v>
       </c>
     </row>
     <row r="43">
@@ -1227,13 +1414,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>17.47</v>
+        <v>34.79</v>
       </c>
       <c r="C43" t="n">
-        <v>23.15</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>21.38</v>
+        <v>16.6</v>
+      </c>
+      <c r="E43" t="n">
+        <v>28.61</v>
       </c>
     </row>
     <row r="44">
@@ -1241,13 +1431,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>17.75</v>
+        <v>34.56</v>
       </c>
       <c r="C44" t="n">
-        <v>23.23</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>22.01</v>
+        <v>16.64</v>
+      </c>
+      <c r="E44" t="n">
+        <v>28.79</v>
       </c>
     </row>
     <row r="45">
@@ -1255,13 +1448,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>18.1</v>
+        <v>34.34</v>
       </c>
       <c r="C45" t="n">
-        <v>23.21</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>22.69</v>
+        <v>16.73</v>
+      </c>
+      <c r="E45" t="n">
+        <v>28.95</v>
       </c>
     </row>
     <row r="46">
@@ -1269,13 +1465,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>18.29</v>
+        <v>34.11</v>
       </c>
       <c r="C46" t="n">
-        <v>23.1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>23.6</v>
+        <v>16.83</v>
+      </c>
+      <c r="E46" t="n">
+        <v>29.11</v>
       </c>
     </row>
     <row r="47">
@@ -1283,13 +1482,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>18.47</v>
+        <v>33.79</v>
       </c>
       <c r="C47" t="n">
-        <v>22.98</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>24.56</v>
+        <v>16.96</v>
+      </c>
+      <c r="E47" t="n">
+        <v>29.31</v>
       </c>
     </row>
     <row r="48">
@@ -1297,13 +1499,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>19.23</v>
+        <v>33.48</v>
       </c>
       <c r="C48" t="n">
-        <v>22.86</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>24.91</v>
+        <v>17.06</v>
+      </c>
+      <c r="E48" t="n">
+        <v>29.54</v>
       </c>
     </row>
     <row r="49">
@@ -1311,13 +1516,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>19.89</v>
+        <v>33.24</v>
       </c>
       <c r="C49" t="n">
-        <v>22.88</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>25.23</v>
+        <v>17.06</v>
+      </c>
+      <c r="E49" t="n">
+        <v>29.8</v>
       </c>
     </row>
     <row r="50">
@@ -1325,13 +1533,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20.54</v>
+        <v>33.27</v>
       </c>
       <c r="C50" t="n">
-        <v>22.94</v>
+        <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>25.52</v>
+        <v>17.26</v>
+      </c>
+      <c r="E50" t="n">
+        <v>29.59</v>
       </c>
     </row>
     <row r="51">
@@ -1339,13 +1550,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>21.2</v>
+        <v>33.3</v>
       </c>
       <c r="C51" t="n">
-        <v>23.02</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>25.78</v>
+        <v>17.47</v>
+      </c>
+      <c r="E51" t="n">
+        <v>29.37</v>
       </c>
     </row>
     <row r="52">
@@ -1353,13 +1567,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20.9</v>
+        <v>33.4</v>
       </c>
       <c r="C52" t="n">
-        <v>23.11</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>25.99</v>
+        <v>17.61</v>
+      </c>
+      <c r="E52" t="n">
+        <v>29.15</v>
       </c>
     </row>
     <row r="53">
@@ -1367,13 +1584,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>20.18</v>
+        <v>33.4</v>
       </c>
       <c r="C53" t="n">
-        <v>23.62</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>26.2</v>
+        <v>17.46</v>
+      </c>
+      <c r="E53" t="n">
+        <v>29.32</v>
       </c>
     </row>
     <row r="54">
@@ -1381,13 +1601,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>19.44</v>
+        <v>33.4</v>
       </c>
       <c r="C54" t="n">
-        <v>24.31</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>26.25</v>
+        <v>17.34</v>
+      </c>
+      <c r="E54" t="n">
+        <v>29.46</v>
       </c>
     </row>
     <row r="55">
@@ -1395,13 +1618,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>18.67</v>
+        <v>33.4</v>
       </c>
       <c r="C55" t="n">
-        <v>25.04</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>26.29</v>
+        <v>17.2</v>
+      </c>
+      <c r="E55" t="n">
+        <v>29.6</v>
       </c>
     </row>
     <row r="56">
@@ -1409,13 +1635,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>18.05</v>
+        <v>33.4</v>
       </c>
       <c r="C56" t="n">
-        <v>25.86</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>26.09</v>
+        <v>17.04</v>
+      </c>
+      <c r="E56" t="n">
+        <v>29.76</v>
       </c>
     </row>
     <row r="57">
@@ -1423,13 +1652,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>17.55</v>
+        <v>33.4</v>
       </c>
       <c r="C57" t="n">
-        <v>26.67</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>25.79</v>
+        <v>16.91</v>
+      </c>
+      <c r="E57" t="n">
+        <v>29.89</v>
       </c>
     </row>
     <row r="58">
@@ -1437,13 +1669,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>17.05</v>
+        <v>33.4</v>
       </c>
       <c r="C58" t="n">
-        <v>27.36</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>25.59</v>
+        <v>16.71</v>
+      </c>
+      <c r="E58" t="n">
+        <v>30.09</v>
       </c>
     </row>
     <row r="59">
@@ -1451,13 +1686,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>16.45</v>
+        <v>33.4</v>
       </c>
       <c r="C59" t="n">
-        <v>27.94</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>25.62</v>
+        <v>16.57</v>
+      </c>
+      <c r="E59" t="n">
+        <v>30.23</v>
       </c>
     </row>
     <row r="60">
@@ -1465,13 +1703,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>15.84</v>
+        <v>33.4</v>
       </c>
       <c r="C60" t="n">
-        <v>28.46</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>25.7</v>
+        <v>16.18</v>
+      </c>
+      <c r="E60" t="n">
+        <v>30.62</v>
       </c>
     </row>
     <row r="61">
@@ -1479,13 +1720,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>15.25</v>
+        <v>33.4</v>
       </c>
       <c r="C61" t="n">
-        <v>28.95</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>25.79</v>
+        <v>15.83</v>
+      </c>
+      <c r="E61" t="n">
+        <v>30.97</v>
       </c>
     </row>
     <row r="62">
@@ -1493,13 +1737,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>14.58</v>
+        <v>33.4</v>
       </c>
       <c r="C62" t="n">
-        <v>29.45</v>
+        <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>25.96</v>
+        <v>15.53</v>
+      </c>
+      <c r="E62" t="n">
+        <v>31.27</v>
       </c>
     </row>
     <row r="63">
@@ -1507,13 +1754,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>14.33</v>
+        <v>33.4</v>
       </c>
       <c r="C63" t="n">
-        <v>29.48</v>
+        <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>26.18</v>
+        <v>15.56</v>
+      </c>
+      <c r="E63" t="n">
+        <v>31.24</v>
       </c>
     </row>
     <row r="64">
@@ -1521,13 +1771,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>14.17</v>
+        <v>33.4</v>
       </c>
       <c r="C64" t="n">
-        <v>29.38</v>
+        <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>26.45</v>
+        <v>15.55</v>
+      </c>
+      <c r="E64" t="n">
+        <v>31.25</v>
       </c>
     </row>
     <row r="65">
@@ -1535,13 +1788,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>13.94</v>
+        <v>33.4</v>
       </c>
       <c r="C65" t="n">
-        <v>29.49</v>
+        <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>26.57</v>
+        <v>15.46</v>
+      </c>
+      <c r="E65" t="n">
+        <v>31.34</v>
       </c>
     </row>
     <row r="66">
@@ -1549,13 +1805,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>13.71</v>
+        <v>33.4</v>
       </c>
       <c r="C66" t="n">
-        <v>29.73</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>26.56</v>
+        <v>15.27</v>
+      </c>
+      <c r="E66" t="n">
+        <v>31.53</v>
       </c>
     </row>
     <row r="67">
@@ -1563,13 +1822,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>13.38</v>
+        <v>33.4</v>
       </c>
       <c r="C67" t="n">
-        <v>29.99</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>26.63</v>
+        <v>15.09</v>
+      </c>
+      <c r="E67" t="n">
+        <v>31.71</v>
       </c>
     </row>
     <row r="68">
@@ -1577,13 +1839,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>13.03</v>
+        <v>33.4</v>
       </c>
       <c r="C68" t="n">
-        <v>30.39</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>26.58</v>
+        <v>14.98</v>
+      </c>
+      <c r="E68" t="n">
+        <v>31.82</v>
       </c>
     </row>
     <row r="69">
@@ -1591,13 +1856,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>12.84</v>
+        <v>33.4</v>
       </c>
       <c r="C69" t="n">
-        <v>30.82</v>
+        <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>26.34</v>
+        <v>14.84</v>
+      </c>
+      <c r="E69" t="n">
+        <v>31.96</v>
       </c>
     </row>
     <row r="70">
@@ -1605,13 +1873,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>12.67</v>
+        <v>33.4</v>
       </c>
       <c r="C70" t="n">
-        <v>31.28</v>
+        <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>26.05</v>
+        <v>14.77</v>
+      </c>
+      <c r="E70" t="n">
+        <v>32.03</v>
       </c>
     </row>
     <row r="71">
@@ -1619,13 +1890,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>12.54</v>
+        <v>33.4</v>
       </c>
       <c r="C71" t="n">
-        <v>31.75</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>25.72</v>
+        <v>14.62</v>
+      </c>
+      <c r="E71" t="n">
+        <v>32.18</v>
       </c>
     </row>
     <row r="72">
@@ -1633,13 +1907,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>12.53</v>
+        <v>33.4</v>
       </c>
       <c r="C72" t="n">
-        <v>32.2</v>
+        <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>25.27</v>
+        <v>14.42</v>
+      </c>
+      <c r="E72" t="n">
+        <v>32.38</v>
       </c>
     </row>
     <row r="73">
@@ -1647,13 +1924,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>12.54</v>
+        <v>33.4</v>
       </c>
       <c r="C73" t="n">
-        <v>32.65</v>
+        <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>24.8</v>
+        <v>14.22</v>
+      </c>
+      <c r="E73" t="n">
+        <v>32.58</v>
       </c>
     </row>
     <row r="74">
@@ -1661,13 +1941,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>12.88</v>
+        <v>33.4</v>
       </c>
       <c r="C74" t="n">
-        <v>32.93</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>24.19</v>
+        <v>14.05</v>
+      </c>
+      <c r="E74" t="n">
+        <v>32.75</v>
       </c>
     </row>
     <row r="75">
@@ -1675,13 +1958,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>13.27</v>
+        <v>33.4</v>
       </c>
       <c r="C75" t="n">
-        <v>32.89</v>
+        <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>23.85</v>
+        <v>13.92</v>
+      </c>
+      <c r="E75" t="n">
+        <v>32.88</v>
       </c>
     </row>
     <row r="76">
@@ -1689,13 +1975,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>13.68</v>
+        <v>33.4</v>
       </c>
       <c r="C76" t="n">
-        <v>32.65</v>
+        <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>23.67</v>
+        <v>13.92</v>
+      </c>
+      <c r="E76" t="n">
+        <v>32.88</v>
       </c>
     </row>
     <row r="77">
@@ -1703,13 +1992,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>13.94</v>
+        <v>33.4</v>
       </c>
       <c r="C77" t="n">
-        <v>32.43</v>
+        <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>23.63</v>
+        <v>13.99</v>
+      </c>
+      <c r="E77" t="n">
+        <v>32.81</v>
       </c>
     </row>
     <row r="78">
@@ -1717,13 +2009,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>14.2</v>
+        <v>33.4</v>
       </c>
       <c r="C78" t="n">
-        <v>32.45</v>
+        <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>23.35</v>
+        <v>14.06</v>
+      </c>
+      <c r="E78" t="n">
+        <v>32.74</v>
       </c>
     </row>
     <row r="79">
@@ -1731,13 +2026,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>14.66</v>
+        <v>33.4</v>
       </c>
       <c r="C79" t="n">
-        <v>32.43</v>
+        <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>22.91</v>
+        <v>14.13</v>
+      </c>
+      <c r="E79" t="n">
+        <v>32.67</v>
       </c>
     </row>
     <row r="80">
@@ -1745,13 +2043,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>15.11</v>
+        <v>33.4</v>
       </c>
       <c r="C80" t="n">
-        <v>32.39</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
-        <v>22.5</v>
+        <v>14.21</v>
+      </c>
+      <c r="E80" t="n">
+        <v>32.59</v>
       </c>
     </row>
     <row r="81">
@@ -1759,13 +2060,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>15.51</v>
+        <v>33.4</v>
       </c>
       <c r="C81" t="n">
-        <v>32.39</v>
+        <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>22.09</v>
+        <v>14.37</v>
+      </c>
+      <c r="E81" t="n">
+        <v>32.43</v>
       </c>
     </row>
     <row r="82">
@@ -1773,13 +2077,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>15.77</v>
+        <v>33.4</v>
       </c>
       <c r="C82" t="n">
-        <v>32.54</v>
+        <v>0</v>
       </c>
       <c r="D82" t="n">
-        <v>21.7</v>
+        <v>14.7</v>
+      </c>
+      <c r="E82" t="n">
+        <v>32.1</v>
       </c>
     </row>
     <row r="83">
@@ -1787,13 +2094,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>16.01</v>
+        <v>33.4</v>
       </c>
       <c r="C83" t="n">
-        <v>32.65</v>
+        <v>0</v>
       </c>
       <c r="D83" t="n">
-        <v>21.35</v>
+        <v>14.99</v>
+      </c>
+      <c r="E83" t="n">
+        <v>31.81</v>
       </c>
     </row>
     <row r="84">
@@ -1801,13 +2111,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>15.84</v>
+        <v>33.4</v>
       </c>
       <c r="C84" t="n">
-        <v>33.02</v>
+        <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>21.14</v>
+        <v>15.28</v>
+      </c>
+      <c r="E84" t="n">
+        <v>31.52</v>
       </c>
     </row>
     <row r="85">
@@ -1815,13 +2128,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>15.68</v>
+        <v>33.4</v>
       </c>
       <c r="C85" t="n">
-        <v>33.69</v>
+        <v>0</v>
       </c>
       <c r="D85" t="n">
-        <v>20.63</v>
+        <v>15.58</v>
+      </c>
+      <c r="E85" t="n">
+        <v>31.22</v>
       </c>
     </row>
     <row r="86">
@@ -1829,13 +2145,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>15.51</v>
+        <v>33.4</v>
       </c>
       <c r="C86" t="n">
-        <v>34.36</v>
+        <v>0</v>
       </c>
       <c r="D86" t="n">
-        <v>20.13</v>
+        <v>15.85</v>
+      </c>
+      <c r="E86" t="n">
+        <v>30.95</v>
       </c>
     </row>
     <row r="87">
@@ -1843,13 +2162,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>15.47</v>
+        <v>33.4</v>
       </c>
       <c r="C87" t="n">
-        <v>35.06</v>
+        <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>19.47</v>
+        <v>16.08</v>
+      </c>
+      <c r="E87" t="n">
+        <v>30.72</v>
       </c>
     </row>
     <row r="88">
@@ -1857,13 +2179,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>15.45</v>
+        <v>33.4</v>
       </c>
       <c r="C88" t="n">
-        <v>35.47</v>
+        <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>19.08</v>
+        <v>16.31</v>
+      </c>
+      <c r="E88" t="n">
+        <v>30.49</v>
       </c>
     </row>
     <row r="89">
@@ -1871,13 +2196,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>15.24</v>
+        <v>33.4</v>
       </c>
       <c r="C89" t="n">
-        <v>35.88</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>18.87</v>
+        <v>16.66</v>
+      </c>
+      <c r="E89" t="n">
+        <v>30.14</v>
       </c>
     </row>
     <row r="90">
@@ -1885,13 +2213,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>15.08</v>
+        <v>33.4</v>
       </c>
       <c r="C90" t="n">
-        <v>36.28</v>
+        <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>18.65</v>
+        <v>17</v>
+      </c>
+      <c r="E90" t="n">
+        <v>29.8</v>
       </c>
     </row>
     <row r="91">
@@ -1899,13 +2230,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>14.92</v>
+        <v>33.4</v>
       </c>
       <c r="C91" t="n">
-        <v>36.63</v>
+        <v>0</v>
       </c>
       <c r="D91" t="n">
-        <v>18.45</v>
+        <v>16.95</v>
+      </c>
+      <c r="E91" t="n">
+        <v>29.86</v>
       </c>
     </row>
     <row r="92">
@@ -1913,13 +2247,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>14.8</v>
+        <v>33.4</v>
       </c>
       <c r="C92" t="n">
-        <v>36.91</v>
+        <v>0</v>
       </c>
       <c r="D92" t="n">
-        <v>18.29</v>
+        <v>16.75</v>
+      </c>
+      <c r="E92" t="n">
+        <v>30.05</v>
       </c>
     </row>
     <row r="93">
@@ -1927,13 +2264,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>14.72</v>
+        <v>33.4</v>
       </c>
       <c r="C93" t="n">
-        <v>37.21</v>
+        <v>0</v>
       </c>
       <c r="D93" t="n">
-        <v>18.07</v>
+        <v>16.57</v>
+      </c>
+      <c r="E93" t="n">
+        <v>30.24</v>
       </c>
     </row>
     <row r="94">
@@ -1941,13 +2281,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>14.72</v>
+        <v>33.4</v>
       </c>
       <c r="C94" t="n">
-        <v>37.45</v>
+        <v>0</v>
       </c>
       <c r="D94" t="n">
-        <v>17.83</v>
+        <v>16.38</v>
+      </c>
+      <c r="E94" t="n">
+        <v>30.42</v>
       </c>
     </row>
     <row r="95">
@@ -1955,13 +2298,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>14.96</v>
+        <v>33.4</v>
       </c>
       <c r="C95" t="n">
-        <v>37.49</v>
+        <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>17.55</v>
+        <v>16.02</v>
+      </c>
+      <c r="E95" t="n">
+        <v>30.78</v>
       </c>
     </row>
     <row r="96">
@@ -1969,13 +2315,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>15.21</v>
+        <v>33.4</v>
       </c>
       <c r="C96" t="n">
-        <v>37.46</v>
+        <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>17.33</v>
+        <v>15.87</v>
+      </c>
+      <c r="E96" t="n">
+        <v>30.93</v>
       </c>
     </row>
     <row r="97">
@@ -1983,13 +2332,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>15.47</v>
+        <v>33.4</v>
       </c>
       <c r="C97" t="n">
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>17.03</v>
+        <v>15.72</v>
+      </c>
+      <c r="E97" t="n">
+        <v>31.09</v>
       </c>
     </row>
     <row r="98">
@@ -1997,13 +2349,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>15.77</v>
+        <v>33.4</v>
       </c>
       <c r="C98" t="n">
-        <v>37.54</v>
+        <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>16.69</v>
+        <v>15.56</v>
+      </c>
+      <c r="E98" t="n">
+        <v>31.24</v>
       </c>
     </row>
     <row r="99">
@@ -2011,13 +2366,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>16.05</v>
+        <v>33.4</v>
       </c>
       <c r="C99" t="n">
-        <v>37.56</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>16.39</v>
+        <v>16.35</v>
+      </c>
+      <c r="E99" t="n">
+        <v>30.46</v>
       </c>
     </row>
     <row r="100">
@@ -2025,13 +2383,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>16.31</v>
+        <v>33.4</v>
       </c>
       <c r="C100" t="n">
-        <v>37.6</v>
+        <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>16.1</v>
+        <v>17.2</v>
+      </c>
+      <c r="E100" t="n">
+        <v>29.6</v>
       </c>
     </row>
     <row r="101">
@@ -2039,13 +2400,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>16.43</v>
+        <v>33.4</v>
       </c>
       <c r="C101" t="n">
-        <v>37.65</v>
+        <v>0</v>
       </c>
       <c r="D101" t="n">
-        <v>15.94</v>
+        <v>18.49</v>
+      </c>
+      <c r="E101" t="n">
+        <v>28.31</v>
       </c>
     </row>
     <row r="102">
@@ -2053,13 +2417,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>16.56</v>
+        <v>33.4</v>
       </c>
       <c r="C102" t="n">
-        <v>37.66</v>
+        <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>15.81</v>
+        <v>19.56</v>
+      </c>
+      <c r="E102" t="n">
+        <v>27.24</v>
       </c>
     </row>
     <row r="103">
@@ -2067,13 +2434,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>16.63</v>
+        <v>33.4</v>
       </c>
       <c r="C103" t="n">
-        <v>37.69</v>
+        <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>15.72</v>
+        <v>20.46</v>
+      </c>
+      <c r="E103" t="n">
+        <v>26.34</v>
       </c>
     </row>
     <row r="104">
@@ -2081,13 +2451,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>16.75</v>
+        <v>33.4</v>
       </c>
       <c r="C104" t="n">
-        <v>37.68</v>
+        <v>0</v>
       </c>
       <c r="D104" t="n">
-        <v>15.62</v>
+        <v>21.43</v>
+      </c>
+      <c r="E104" t="n">
+        <v>25.37</v>
       </c>
     </row>
     <row r="105">
@@ -2095,13 +2468,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>16.51</v>
+        <v>33.4</v>
       </c>
       <c r="C105" t="n">
-        <v>37.66</v>
+        <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>15.88</v>
+        <v>22.57</v>
+      </c>
+      <c r="E105" t="n">
+        <v>24.23</v>
       </c>
     </row>
     <row r="106">
@@ -2109,13 +2485,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>16.28</v>
+        <v>33.4</v>
       </c>
       <c r="C106" t="n">
-        <v>37.68</v>
+        <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>16.09</v>
+        <v>23.47</v>
+      </c>
+      <c r="E106" t="n">
+        <v>23.33</v>
       </c>
     </row>
     <row r="107">
@@ -2123,13 +2502,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>16.13</v>
+        <v>33.4</v>
       </c>
       <c r="C107" t="n">
-        <v>37.54</v>
+        <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>16.38</v>
+        <v>24.37</v>
+      </c>
+      <c r="E107" t="n">
+        <v>22.43</v>
       </c>
     </row>
     <row r="108">
@@ -2137,13 +2519,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>15.93</v>
+        <v>33.4</v>
       </c>
       <c r="C108" t="n">
-        <v>37.51</v>
+        <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>16.61</v>
+        <v>25.32</v>
+      </c>
+      <c r="E108" t="n">
+        <v>21.48</v>
       </c>
     </row>
     <row r="109">
@@ -2151,13 +2536,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>15.73</v>
+        <v>33.38</v>
       </c>
       <c r="C109" t="n">
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>16.82</v>
+        <v>25.21</v>
+      </c>
+      <c r="E109" t="n">
+        <v>21.59</v>
       </c>
     </row>
     <row r="110">
@@ -2165,13 +2553,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>15.52</v>
+        <v>33.52</v>
       </c>
       <c r="C110" t="n">
-        <v>37.48</v>
+        <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>17.04</v>
+        <v>24.86</v>
+      </c>
+      <c r="E110" t="n">
+        <v>21.78</v>
       </c>
     </row>
     <row r="111">
@@ -2179,13 +2570,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>15.48</v>
+        <v>33.66</v>
       </c>
       <c r="C111" t="n">
-        <v>37.45</v>
+        <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>17.1</v>
+        <v>24.44</v>
+      </c>
+      <c r="E111" t="n">
+        <v>22.04</v>
       </c>
     </row>
     <row r="112">
@@ -2193,13 +2587,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>15.46</v>
+        <v>33.98</v>
       </c>
       <c r="C112" t="n">
-        <v>37.4</v>
+        <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>17.16</v>
+        <v>24.11</v>
+      </c>
+      <c r="E112" t="n">
+        <v>22.03</v>
       </c>
     </row>
     <row r="113">
@@ -2207,13 +2604,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>15.45</v>
+        <v>34.36</v>
       </c>
       <c r="C113" t="n">
-        <v>37.31</v>
+        <v>0</v>
       </c>
       <c r="D113" t="n">
-        <v>17.24</v>
+        <v>23.9</v>
+      </c>
+      <c r="E113" t="n">
+        <v>21.84</v>
       </c>
     </row>
     <row r="114">
@@ -2221,13 +2621,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>15.33</v>
+        <v>34.27</v>
       </c>
       <c r="C114" t="n">
-        <v>37.21</v>
+        <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>17.45</v>
+        <v>24.1</v>
+      </c>
+      <c r="E114" t="n">
+        <v>21.71</v>
       </c>
     </row>
     <row r="115">
@@ -2235,13 +2638,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>15.28</v>
+        <v>34.36</v>
       </c>
       <c r="C115" t="n">
-        <v>37.11</v>
+        <v>0</v>
       </c>
       <c r="D115" t="n">
-        <v>17.62</v>
+        <v>24.31</v>
+      </c>
+      <c r="E115" t="n">
+        <v>21.39</v>
       </c>
     </row>
     <row r="116">
@@ -2249,13 +2655,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>15.2</v>
+        <v>34.75</v>
       </c>
       <c r="C116" t="n">
-        <v>37.01</v>
+        <v>0</v>
       </c>
       <c r="D116" t="n">
-        <v>17.79</v>
+        <v>24.34</v>
+      </c>
+      <c r="E116" t="n">
+        <v>20.95</v>
       </c>
     </row>
     <row r="117">
@@ -2263,13 +2672,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>15.14</v>
+        <v>35.08</v>
       </c>
       <c r="C117" t="n">
-        <v>36.96</v>
+        <v>0</v>
       </c>
       <c r="D117" t="n">
-        <v>17.9</v>
+        <v>24.29</v>
+      </c>
+      <c r="E117" t="n">
+        <v>20.65</v>
       </c>
     </row>
     <row r="118">
@@ -2277,13 +2689,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>15.11</v>
+        <v>35.72</v>
       </c>
       <c r="C118" t="n">
-        <v>36.83</v>
+        <v>0</v>
       </c>
       <c r="D118" t="n">
-        <v>18.06</v>
+        <v>23.88</v>
+      </c>
+      <c r="E118" t="n">
+        <v>20.4</v>
       </c>
     </row>
     <row r="119">
@@ -2291,13 +2706,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>15.03</v>
+        <v>36.18</v>
       </c>
       <c r="C119" t="n">
-        <v>36.67</v>
+        <v>0</v>
       </c>
       <c r="D119" t="n">
-        <v>18.3</v>
+        <v>23.65</v>
+      </c>
+      <c r="E119" t="n">
+        <v>20.17</v>
       </c>
     </row>
     <row r="120">
@@ -2305,13 +2723,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>14.99</v>
+        <v>36.48</v>
       </c>
       <c r="C120" t="n">
-        <v>36.49</v>
+        <v>0</v>
       </c>
       <c r="D120" t="n">
-        <v>18.52</v>
+        <v>23.64</v>
+      </c>
+      <c r="E120" t="n">
+        <v>19.88</v>
       </c>
     </row>
     <row r="121">
@@ -2319,13 +2740,16 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>14.92</v>
+        <v>37.12</v>
       </c>
       <c r="C121" t="n">
-        <v>36.31</v>
+        <v>0</v>
       </c>
       <c r="D121" t="n">
-        <v>18.77</v>
+        <v>23.37</v>
+      </c>
+      <c r="E121" t="n">
+        <v>19.51</v>
       </c>
     </row>
     <row r="122">
@@ -2333,13 +2757,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>14.94</v>
+        <v>37.57</v>
       </c>
       <c r="C122" t="n">
-        <v>36.14</v>
+        <v>0</v>
       </c>
       <c r="D122" t="n">
-        <v>18.92</v>
+        <v>23.17</v>
+      </c>
+      <c r="E122" t="n">
+        <v>19.26</v>
       </c>
     </row>
     <row r="123">
@@ -2347,13 +2774,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>15.26</v>
+        <v>37.88</v>
       </c>
       <c r="C123" t="n">
-        <v>35.8</v>
+        <v>0</v>
       </c>
       <c r="D123" t="n">
-        <v>18.94</v>
+        <v>23.19</v>
+      </c>
+      <c r="E123" t="n">
+        <v>18.93</v>
       </c>
     </row>
     <row r="124">
@@ -2361,13 +2791,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>15.64</v>
+        <v>37.21</v>
       </c>
       <c r="C124" t="n">
-        <v>35.46</v>
+        <v>0</v>
       </c>
       <c r="D124" t="n">
-        <v>18.9</v>
+        <v>24.18</v>
+      </c>
+      <c r="E124" t="n">
+        <v>18.61</v>
       </c>
     </row>
     <row r="125">
@@ -2375,13 +2808,16 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>16.06</v>
+        <v>36.38</v>
       </c>
       <c r="C125" t="n">
-        <v>35.17</v>
+        <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>18.77</v>
+        <v>25.15</v>
+      </c>
+      <c r="E125" t="n">
+        <v>18.47</v>
       </c>
     </row>
     <row r="126">
@@ -2389,13 +2825,16 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>16.49</v>
+        <v>35.25</v>
       </c>
       <c r="C126" t="n">
-        <v>34.88</v>
+        <v>0</v>
       </c>
       <c r="D126" t="n">
-        <v>18.63</v>
+        <v>26.38</v>
+      </c>
+      <c r="E126" t="n">
+        <v>18.37</v>
       </c>
     </row>
     <row r="127">
@@ -2403,13 +2842,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>16.82</v>
+        <v>34.11</v>
       </c>
       <c r="C127" t="n">
-        <v>34.6</v>
+        <v>0</v>
       </c>
       <c r="D127" t="n">
-        <v>18.59</v>
+        <v>27.6</v>
+      </c>
+      <c r="E127" t="n">
+        <v>18.29</v>
       </c>
     </row>
     <row r="128">
@@ -2417,13 +2859,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>17.19</v>
+        <v>32.21</v>
       </c>
       <c r="C128" t="n">
-        <v>34.27</v>
+        <v>0</v>
       </c>
       <c r="D128" t="n">
-        <v>18.54</v>
+        <v>29.57</v>
+      </c>
+      <c r="E128" t="n">
+        <v>18.22</v>
       </c>
     </row>
     <row r="129">
@@ -2431,13 +2876,16 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>17.55</v>
+        <v>30.75</v>
       </c>
       <c r="C129" t="n">
-        <v>34.01</v>
+        <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>18.43</v>
+        <v>31.12</v>
+      </c>
+      <c r="E129" t="n">
+        <v>18.13</v>
       </c>
     </row>
     <row r="130">
@@ -2445,13 +2893,16 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>17.96</v>
+        <v>29.08</v>
       </c>
       <c r="C130" t="n">
-        <v>33.76</v>
+        <v>0</v>
       </c>
       <c r="D130" t="n">
-        <v>18.27</v>
+        <v>32.62</v>
+      </c>
+      <c r="E130" t="n">
+        <v>18.3</v>
       </c>
     </row>
     <row r="131">
@@ -2459,13 +2910,16 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>18.1</v>
+        <v>26.98</v>
       </c>
       <c r="C131" t="n">
-        <v>33.53</v>
+        <v>0</v>
       </c>
       <c r="D131" t="n">
-        <v>18.37</v>
+        <v>34.48</v>
+      </c>
+      <c r="E131" t="n">
+        <v>18.54</v>
       </c>
     </row>
     <row r="132">
@@ -2473,13 +2927,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>18.09</v>
+        <v>26.6</v>
       </c>
       <c r="C132" t="n">
-        <v>33.38</v>
+        <v>0</v>
       </c>
       <c r="D132" t="n">
-        <v>18.53</v>
+        <v>34.67</v>
+      </c>
+      <c r="E132" t="n">
+        <v>18.73</v>
       </c>
     </row>
     <row r="133">
@@ -2487,13 +2944,16 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>17.81</v>
+        <v>26.25</v>
       </c>
       <c r="C133" t="n">
-        <v>33.43</v>
+        <v>0</v>
       </c>
       <c r="D133" t="n">
-        <v>18.76</v>
+        <v>34.77</v>
+      </c>
+      <c r="E133" t="n">
+        <v>18.99</v>
       </c>
     </row>
     <row r="134">
@@ -2501,13 +2961,16 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>17.59</v>
+        <v>27.77</v>
       </c>
       <c r="C134" t="n">
-        <v>33.48</v>
+        <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>18.93</v>
+        <v>33.4</v>
+      </c>
+      <c r="E134" t="n">
+        <v>19.26</v>
       </c>
     </row>
     <row r="135">
@@ -2515,13 +2978,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>17.38</v>
+        <v>29.36</v>
       </c>
       <c r="C135" t="n">
-        <v>33.12</v>
+        <v>0</v>
       </c>
       <c r="D135" t="n">
-        <v>19.49</v>
+        <v>32.05</v>
+      </c>
+      <c r="E135" t="n">
+        <v>19.45</v>
       </c>
     </row>
     <row r="136">
@@ -2529,13 +2995,16 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>17.18</v>
+        <v>31.62</v>
       </c>
       <c r="C136" t="n">
-        <v>32.78</v>
+        <v>0</v>
       </c>
       <c r="D136" t="n">
-        <v>20.04</v>
+        <v>30.69</v>
+      </c>
+      <c r="E136" t="n">
+        <v>18.98</v>
       </c>
     </row>
     <row r="137">
@@ -2543,13 +3012,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>16.96</v>
+        <v>33.97</v>
       </c>
       <c r="C137" t="n">
-        <v>32.45</v>
+        <v>0</v>
       </c>
       <c r="D137" t="n">
-        <v>20.6</v>
+        <v>29.39</v>
+      </c>
+      <c r="E137" t="n">
+        <v>18.35</v>
       </c>
     </row>
     <row r="138">
@@ -2557,13 +3029,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>16.55</v>
+        <v>36.79</v>
       </c>
       <c r="C138" t="n">
-        <v>32.11</v>
+        <v>0</v>
       </c>
       <c r="D138" t="n">
-        <v>21.34</v>
+        <v>27.22</v>
+      </c>
+      <c r="E138" t="n">
+        <v>17.71</v>
       </c>
     </row>
     <row r="139">
@@ -2571,13 +3046,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>16.19</v>
+        <v>39.37</v>
       </c>
       <c r="C139" t="n">
-        <v>31.77</v>
+        <v>0</v>
       </c>
       <c r="D139" t="n">
-        <v>22.04</v>
+        <v>25.28</v>
+      </c>
+      <c r="E139" t="n">
+        <v>17.07</v>
       </c>
     </row>
     <row r="140">
@@ -2585,13 +3063,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>15.72</v>
+        <v>42.07</v>
       </c>
       <c r="C140" t="n">
-        <v>31.45</v>
+        <v>0</v>
       </c>
       <c r="D140" t="n">
-        <v>22.83</v>
+        <v>23.26</v>
+      </c>
+      <c r="E140" t="n">
+        <v>16.39</v>
       </c>
     </row>
     <row r="141">
@@ -2599,13 +3080,19 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>15.52</v>
+        <v>44.39</v>
       </c>
       <c r="C141" t="n">
-        <v>31.11</v>
+        <v>0</v>
       </c>
       <c r="D141" t="n">
-        <v>23.38</v>
+        <v>21.62</v>
+      </c>
+      <c r="E141" t="n">
+        <v>15.71</v>
+      </c>
+      <c r="F141" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="142">
@@ -2613,13 +3100,19 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>15.36</v>
+        <v>44.81</v>
       </c>
       <c r="C142" t="n">
-        <v>30.66</v>
+        <v>0</v>
       </c>
       <c r="D142" t="n">
-        <v>23.98</v>
+        <v>22.58</v>
+      </c>
+      <c r="E142" t="n">
+        <v>14.33</v>
+      </c>
+      <c r="F142" t="n">
+        <v>19.715</v>
       </c>
     </row>
     <row r="143">
@@ -2627,13 +3120,19 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>15.25</v>
+        <v>45.23</v>
       </c>
       <c r="C143" t="n">
-        <v>30.23</v>
+        <v>0</v>
       </c>
       <c r="D143" t="n">
-        <v>24.53</v>
+        <v>23.41</v>
+      </c>
+      <c r="E143" t="n">
+        <v>13.13</v>
+      </c>
+      <c r="F143" t="n">
+        <v>19.55333333333333</v>
       </c>
     </row>
     <row r="144">
@@ -2641,13 +3140,19 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>15</v>
+        <v>45.27</v>
       </c>
       <c r="C144" t="n">
-        <v>29.88</v>
+        <v>0</v>
       </c>
       <c r="D144" t="n">
-        <v>25.12</v>
+        <v>24.23</v>
+      </c>
+      <c r="E144" t="n">
+        <v>11.93</v>
+      </c>
+      <c r="F144" t="n">
+        <v>19.4475</v>
       </c>
     </row>
     <row r="145">
@@ -2655,13 +3160,19 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>14.77</v>
+        <v>45.48</v>
       </c>
       <c r="C145" t="n">
-        <v>29.89</v>
+        <v>0</v>
       </c>
       <c r="D145" t="n">
-        <v>25.34</v>
+        <v>24.79</v>
+      </c>
+      <c r="E145" t="n">
+        <v>10.81</v>
+      </c>
+      <c r="F145" t="n">
+        <v>19.384</v>
       </c>
     </row>
     <row r="146">
@@ -2669,13 +3180,19 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>14.47</v>
+        <v>45.01</v>
       </c>
       <c r="C146" t="n">
-        <v>30.05</v>
+        <v>0</v>
       </c>
       <c r="D146" t="n">
-        <v>25.48</v>
+        <v>25.31</v>
+      </c>
+      <c r="E146" t="n">
+        <v>10.41</v>
+      </c>
+      <c r="F146" t="n">
+        <v>18.96166666666667</v>
       </c>
     </row>
     <row r="147">
@@ -2683,13 +3200,19 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>14.21</v>
+        <v>44.47</v>
       </c>
       <c r="C147" t="n">
-        <v>30.19</v>
+        <v>0</v>
       </c>
       <c r="D147" t="n">
-        <v>25.6</v>
+        <v>25.78</v>
+      </c>
+      <c r="E147" t="n">
+        <v>10.38</v>
+      </c>
+      <c r="F147" t="n">
+        <v>18.53142857142857</v>
       </c>
     </row>
     <row r="148">
@@ -2697,13 +3220,19 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>14.16</v>
+        <v>43.9</v>
       </c>
       <c r="C148" t="n">
-        <v>30.34</v>
+        <v>0</v>
       </c>
       <c r="D148" t="n">
-        <v>25.5</v>
+        <v>26.77</v>
+      </c>
+      <c r="E148" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="F148" t="n">
+        <v>18.23375</v>
       </c>
     </row>
     <row r="149">
@@ -2711,13 +3240,19 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>14.12</v>
+        <v>43.34</v>
       </c>
       <c r="C149" t="n">
-        <v>30.47</v>
+        <v>0</v>
       </c>
       <c r="D149" t="n">
-        <v>25.43</v>
+        <v>27.73</v>
+      </c>
+      <c r="E149" t="n">
+        <v>10.34</v>
+      </c>
+      <c r="F149" t="n">
+        <v>17.93555555555555</v>
       </c>
     </row>
     <row r="150">
@@ -2725,13 +3260,19 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>14.11</v>
+        <v>42.8</v>
       </c>
       <c r="C150" t="n">
-        <v>30.62</v>
+        <v>0</v>
       </c>
       <c r="D150" t="n">
-        <v>25.31</v>
+        <v>28.91</v>
+      </c>
+      <c r="E150" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="F150" t="n">
+        <v>16.512</v>
       </c>
     </row>
     <row r="151">
@@ -2739,13 +3280,19 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>15.23</v>
+        <v>42.68</v>
       </c>
       <c r="C151" t="n">
-        <v>29.66</v>
+        <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>25.14</v>
+        <v>29.6</v>
+      </c>
+      <c r="E151" t="n">
+        <v>11.21</v>
+      </c>
+      <c r="F151" t="n">
+        <v>16.512</v>
       </c>
     </row>
     <row r="152">
@@ -2753,13 +3300,19 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>16.36</v>
+        <v>42.85</v>
       </c>
       <c r="C152" t="n">
-        <v>28.75</v>
+        <v>0</v>
       </c>
       <c r="D152" t="n">
-        <v>24.93</v>
+        <v>29.34</v>
+      </c>
+      <c r="E152" t="n">
+        <v>12.99</v>
+      </c>
+      <c r="F152" t="n">
+        <v>14.822</v>
       </c>
     </row>
     <row r="153">
@@ -2767,13 +3320,19 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>17.41</v>
+        <v>43.98</v>
       </c>
       <c r="C153" t="n">
-        <v>27.88</v>
+        <v>0</v>
       </c>
       <c r="D153" t="n">
-        <v>24.76</v>
+        <v>28.31</v>
+      </c>
+      <c r="E153" t="n">
+        <v>14.53</v>
+      </c>
+      <c r="F153" t="n">
+        <v>13.179</v>
       </c>
     </row>
     <row r="154">
@@ -2781,13 +3340,19 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>18.55</v>
+        <v>45.21</v>
       </c>
       <c r="C154" t="n">
-        <v>26.91</v>
+        <v>0</v>
       </c>
       <c r="D154" t="n">
-        <v>24.58</v>
+        <v>27.24</v>
+      </c>
+      <c r="E154" t="n">
+        <v>15.99</v>
+      </c>
+      <c r="F154" t="n">
+        <v>11.556</v>
       </c>
     </row>
     <row r="155">
@@ -2795,13 +3360,19 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>19.63</v>
+        <v>45.84</v>
       </c>
       <c r="C155" t="n">
-        <v>25.95</v>
+        <v>0</v>
       </c>
       <c r="D155" t="n">
-        <v>24.46</v>
+        <v>26.41</v>
+      </c>
+      <c r="E155" t="n">
+        <v>17.81</v>
+      </c>
+      <c r="F155" t="n">
+        <v>9.943000000000001</v>
       </c>
     </row>
     <row r="156">
@@ -2809,13 +3380,19 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>20.82</v>
+        <v>46.5</v>
       </c>
       <c r="C156" t="n">
-        <v>24.82</v>
+        <v>0</v>
       </c>
       <c r="D156" t="n">
-        <v>24.4</v>
+        <v>25.61</v>
+      </c>
+      <c r="E156" t="n">
+        <v>19.58</v>
+      </c>
+      <c r="F156" t="n">
+        <v>8.309999999999999</v>
       </c>
     </row>
     <row r="157">
@@ -2823,13 +3400,19 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>22.04</v>
+        <v>47.3</v>
       </c>
       <c r="C157" t="n">
-        <v>23.66</v>
+        <v>0</v>
       </c>
       <c r="D157" t="n">
-        <v>24.33</v>
+        <v>24.79</v>
+      </c>
+      <c r="E157" t="n">
+        <v>21.01</v>
+      </c>
+      <c r="F157" t="n">
+        <v>6.895</v>
       </c>
     </row>
     <row r="158">
@@ -2837,13 +3420,19 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>23.2</v>
+        <v>48.11</v>
       </c>
       <c r="C158" t="n">
-        <v>22.51</v>
+        <v>0</v>
       </c>
       <c r="D158" t="n">
-        <v>24.33</v>
+        <v>23.95</v>
+      </c>
+      <c r="E158" t="n">
+        <v>22.43</v>
+      </c>
+      <c r="F158" t="n">
+        <v>5.513</v>
       </c>
     </row>
     <row r="159">
@@ -2851,13 +3440,19 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>24.32</v>
+        <v>49.02</v>
       </c>
       <c r="C159" t="n">
-        <v>21.4</v>
+        <v>0</v>
       </c>
       <c r="D159" t="n">
-        <v>24.31</v>
+        <v>21.1</v>
+      </c>
+      <c r="E159" t="n">
+        <v>23.83</v>
+      </c>
+      <c r="F159" t="n">
+        <v>4.111</v>
       </c>
     </row>
     <row r="160">
@@ -2865,13 +3460,19 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>25.58</v>
+        <v>50.08</v>
       </c>
       <c r="C160" t="n">
-        <v>20.2</v>
+        <v>0</v>
       </c>
       <c r="D160" t="n">
-        <v>24.23</v>
+        <v>20.05</v>
+      </c>
+      <c r="E160" t="n">
+        <v>25.17</v>
+      </c>
+      <c r="F160" t="n">
+        <v>2.749</v>
       </c>
     </row>
     <row r="161">
@@ -2879,13 +3480,19 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>25.72</v>
+        <v>51.2</v>
       </c>
       <c r="C161" t="n">
-        <v>20.14</v>
+        <v>0</v>
       </c>
       <c r="D161" t="n">
-        <v>24.14</v>
+        <v>18.99</v>
+      </c>
+      <c r="E161" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="F161" t="n">
+        <v>4.561999999999999</v>
       </c>
     </row>
     <row r="162">
@@ -2893,13 +3500,19 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>25.88</v>
+        <v>52.69</v>
       </c>
       <c r="C162" t="n">
-        <v>20.06</v>
+        <v>0</v>
       </c>
       <c r="D162" t="n">
-        <v>24.05</v>
+        <v>17.97</v>
+      </c>
+      <c r="E162" t="n">
+        <v>25.42</v>
+      </c>
+      <c r="F162" t="n">
+        <v>5.976</v>
       </c>
     </row>
     <row r="163">
@@ -2907,13 +3520,19 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>25.7</v>
+        <v>53.27</v>
       </c>
       <c r="C163" t="n">
-        <v>19.88</v>
+        <v>0</v>
       </c>
       <c r="D163" t="n">
-        <v>24.41</v>
+        <v>17.67</v>
+      </c>
+      <c r="E163" t="n">
+        <v>25.72</v>
+      </c>
+      <c r="F163" t="n">
+        <v>7.4</v>
       </c>
     </row>
     <row r="164">
@@ -2921,13 +3540,19 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>25.49</v>
+        <v>53.7</v>
       </c>
       <c r="C164" t="n">
-        <v>19.76</v>
+        <v>0</v>
       </c>
       <c r="D164" t="n">
-        <v>24.75</v>
+        <v>17.45</v>
+      </c>
+      <c r="E164" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="F164" t="n">
+        <v>8.803999999999998</v>
       </c>
     </row>
     <row r="165">
@@ -2935,13 +3560,19 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>25.17</v>
+        <v>54.97</v>
       </c>
       <c r="C165" t="n">
-        <v>19.98</v>
+        <v>0</v>
       </c>
       <c r="D165" t="n">
-        <v>24.85</v>
+        <v>16.78</v>
+      </c>
+      <c r="E165" t="n">
+        <v>26.11</v>
+      </c>
+      <c r="F165" t="n">
+        <v>10.198</v>
       </c>
     </row>
     <row r="166">
@@ -2949,13 +3580,19 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>24.8</v>
+        <v>56.22</v>
       </c>
       <c r="C166" t="n">
-        <v>20.24</v>
+        <v>0</v>
       </c>
       <c r="D166" t="n">
-        <v>24.96</v>
+        <v>16.09</v>
+      </c>
+      <c r="E166" t="n">
+        <v>26.16</v>
+      </c>
+      <c r="F166" t="n">
+        <v>11.592</v>
       </c>
     </row>
     <row r="167">
@@ -2963,13 +3600,19 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>24.38</v>
+        <v>57.29</v>
       </c>
       <c r="C167" t="n">
-        <v>20.56</v>
+        <v>0</v>
       </c>
       <c r="D167" t="n">
-        <v>25.06</v>
+        <v>15.63</v>
+      </c>
+      <c r="E167" t="n">
+        <v>26.13</v>
+      </c>
+      <c r="F167" t="n">
+        <v>12.996</v>
       </c>
     </row>
     <row r="168">
@@ -2977,13 +3620,19 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>23.9</v>
+        <v>58.36</v>
       </c>
       <c r="C168" t="n">
-        <v>20.82</v>
+        <v>0</v>
       </c>
       <c r="D168" t="n">
-        <v>25.28</v>
+        <v>15.18</v>
+      </c>
+      <c r="E168" t="n">
+        <v>26.12</v>
+      </c>
+      <c r="F168" t="n">
+        <v>14.387</v>
       </c>
     </row>
     <row r="169">
@@ -2991,13 +3640,19 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>23.34</v>
+        <v>59.34</v>
       </c>
       <c r="C169" t="n">
-        <v>21.13</v>
+        <v>0</v>
       </c>
       <c r="D169" t="n">
-        <v>25.53</v>
+        <v>16.84</v>
+      </c>
+      <c r="E169" t="n">
+        <v>26.12</v>
+      </c>
+      <c r="F169" t="n">
+        <v>15.768</v>
       </c>
     </row>
     <row r="170">
@@ -3005,13 +3660,19 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>22.64</v>
+        <v>60.3</v>
       </c>
       <c r="C170" t="n">
-        <v>21.51</v>
+        <v>0</v>
       </c>
       <c r="D170" t="n">
-        <v>25.85</v>
+        <v>16.47</v>
+      </c>
+      <c r="E170" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="F170" t="n">
+        <v>17.169</v>
       </c>
     </row>
     <row r="171">
@@ -3019,13 +3680,19 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>22</v>
+        <v>61.2</v>
       </c>
       <c r="C171" t="n">
-        <v>21.86</v>
+        <v>0</v>
       </c>
       <c r="D171" t="n">
-        <v>26.14</v>
+        <v>16.18</v>
+      </c>
+      <c r="E171" t="n">
+        <v>26.25</v>
+      </c>
+      <c r="F171" t="n">
+        <v>16.58</v>
       </c>
     </row>
     <row r="172">
@@ -3033,13 +3700,19 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>21.33</v>
+        <v>62.23</v>
       </c>
       <c r="C172" t="n">
-        <v>22.2</v>
+        <v>0</v>
       </c>
       <c r="D172" t="n">
-        <v>26.47</v>
+        <v>15.31</v>
+      </c>
+      <c r="E172" t="n">
+        <v>26.31</v>
+      </c>
+      <c r="F172" t="n">
+        <v>16.43</v>
       </c>
     </row>
     <row r="173">
@@ -3047,13 +3720,19 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>21.01</v>
+        <v>63.06</v>
       </c>
       <c r="C173" t="n">
-        <v>22.66</v>
+        <v>0</v>
       </c>
       <c r="D173" t="n">
-        <v>26.33</v>
+        <v>14.54</v>
+      </c>
+      <c r="E173" t="n">
+        <v>26.25</v>
+      </c>
+      <c r="F173" t="n">
+        <v>16.52</v>
       </c>
     </row>
     <row r="174">
@@ -3061,13 +3740,19 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>20.7</v>
+        <v>63.92</v>
       </c>
       <c r="C174" t="n">
-        <v>23.05</v>
+        <v>0</v>
       </c>
       <c r="D174" t="n">
-        <v>26.25</v>
+        <v>13.72</v>
+      </c>
+      <c r="E174" t="n">
+        <v>26.19</v>
+      </c>
+      <c r="F174" t="n">
+        <v>16.61</v>
       </c>
     </row>
     <row r="175">
@@ -3075,13 +3760,19 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>20.48</v>
+        <v>64.27</v>
       </c>
       <c r="C175" t="n">
-        <v>23.11</v>
+        <v>0</v>
       </c>
       <c r="D175" t="n">
-        <v>26.41</v>
+        <v>13.31</v>
+      </c>
+      <c r="E175" t="n">
+        <v>26.15</v>
+      </c>
+      <c r="F175" t="n">
+        <v>16.777</v>
       </c>
     </row>
     <row r="176">
@@ -3089,13 +3780,19 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>20.38</v>
+        <v>64.72</v>
       </c>
       <c r="C176" t="n">
-        <v>23.08</v>
+        <v>0</v>
       </c>
       <c r="D176" t="n">
-        <v>26.54</v>
+        <v>12.85</v>
+      </c>
+      <c r="E176" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F176" t="n">
+        <v>16.944</v>
       </c>
     </row>
     <row r="177">
@@ -3103,13 +3800,19 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>20.26</v>
+        <v>65.38</v>
       </c>
       <c r="C177" t="n">
-        <v>23.05</v>
+        <v>0</v>
       </c>
       <c r="D177" t="n">
-        <v>26.69</v>
+        <v>12.15</v>
+      </c>
+      <c r="E177" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F177" t="n">
+        <v>17.046</v>
       </c>
     </row>
     <row r="178">
@@ -3117,13 +3820,19 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>20.2</v>
+        <v>66.28</v>
       </c>
       <c r="C178" t="n">
-        <v>23.06</v>
+        <v>0</v>
       </c>
       <c r="D178" t="n">
-        <v>26.74</v>
+        <v>11.36</v>
+      </c>
+      <c r="E178" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F178" t="n">
+        <v>17.003</v>
       </c>
     </row>
     <row r="179">
@@ -3131,13 +3840,19 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>20.24</v>
+        <v>67.17</v>
       </c>
       <c r="C179" t="n">
-        <v>23.03</v>
+        <v>0</v>
       </c>
       <c r="D179" t="n">
-        <v>26.73</v>
+        <v>10.55</v>
+      </c>
+      <c r="E179" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F179" t="n">
+        <v>16.925</v>
       </c>
     </row>
     <row r="180">
@@ -3145,13 +3860,19 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>20.26</v>
+        <v>68.15000000000001</v>
       </c>
       <c r="C180" t="n">
-        <v>22.89</v>
+        <v>0</v>
       </c>
       <c r="D180" t="n">
-        <v>26.85</v>
+        <v>9.68</v>
+      </c>
+      <c r="E180" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F180" t="n">
+        <v>16.827</v>
       </c>
     </row>
     <row r="181">
@@ -3159,13 +3880,19 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>20.42</v>
+        <v>69.18000000000001</v>
       </c>
       <c r="C181" t="n">
-        <v>22.73</v>
+        <v>0</v>
       </c>
       <c r="D181" t="n">
-        <v>26.85</v>
+        <v>8.76</v>
+      </c>
+      <c r="E181" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F181" t="n">
+        <v>16.709</v>
       </c>
     </row>
     <row r="182">
@@ -3173,13 +3900,19 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>20.59</v>
+        <v>69.53</v>
       </c>
       <c r="C182" t="n">
-        <v>22.58</v>
+        <v>0</v>
       </c>
       <c r="D182" t="n">
-        <v>26.83</v>
+        <v>8.5</v>
+      </c>
+      <c r="E182" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F182" t="n">
+        <v>16.611</v>
       </c>
     </row>
     <row r="183">
@@ -3187,13 +3920,19 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>20.78</v>
+        <v>70.33</v>
       </c>
       <c r="C183" t="n">
-        <v>22.37</v>
+        <v>0</v>
       </c>
       <c r="D183" t="n">
-        <v>26.86</v>
+        <v>8.050000000000001</v>
+      </c>
+      <c r="E183" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F183" t="n">
+        <v>16.253</v>
       </c>
     </row>
     <row r="184">
@@ -3201,13 +3940,19 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>20.98</v>
+        <v>71.09999999999999</v>
       </c>
       <c r="C184" t="n">
-        <v>22.21</v>
+        <v>0</v>
       </c>
       <c r="D184" t="n">
-        <v>26.82</v>
+        <v>7.49</v>
+      </c>
+      <c r="E184" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F184" t="n">
+        <v>16.035</v>
       </c>
     </row>
     <row r="185">
@@ -3215,13 +3960,19 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>21.24</v>
+        <v>72.36</v>
       </c>
       <c r="C185" t="n">
-        <v>22.09</v>
+        <v>0</v>
       </c>
       <c r="D185" t="n">
-        <v>26.67</v>
+        <v>6.54</v>
+      </c>
+      <c r="E185" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F185" t="n">
+        <v>15.73</v>
       </c>
     </row>
     <row r="186">
@@ -3229,13 +3980,19 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>21.41</v>
+        <v>74.84999999999999</v>
       </c>
       <c r="C186" t="n">
-        <v>22.02</v>
+        <v>0</v>
       </c>
       <c r="D186" t="n">
-        <v>26.57</v>
+        <v>5.67</v>
+      </c>
+      <c r="E186" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F186" t="n">
+        <v>14.105</v>
       </c>
     </row>
     <row r="187">
@@ -3243,13 +4000,19 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>21.7</v>
+        <v>77.23</v>
       </c>
       <c r="C187" t="n">
-        <v>21.94</v>
+        <v>0</v>
       </c>
       <c r="D187" t="n">
-        <v>26.36</v>
+        <v>4.87</v>
+      </c>
+      <c r="E187" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F187" t="n">
+        <v>12.535</v>
       </c>
     </row>
     <row r="188">
@@ -3257,13 +4020,19 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>22</v>
+        <v>79.37</v>
       </c>
       <c r="C188" t="n">
-        <v>21.86</v>
+        <v>0</v>
       </c>
       <c r="D188" t="n">
-        <v>26.14</v>
+        <v>4.08</v>
+      </c>
+      <c r="E188" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F188" t="n">
+        <v>11.18</v>
       </c>
     </row>
     <row r="189">
@@ -3271,545 +4040,19 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>22.28</v>
+        <v>81.54000000000001</v>
       </c>
       <c r="C189" t="n">
-        <v>21.77</v>
+        <v>0</v>
       </c>
       <c r="D189" t="n">
-        <v>25.95</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" s="1" t="n">
-        <v>188</v>
-      </c>
-      <c r="B190" t="n">
-        <v>22.57</v>
-      </c>
-      <c r="C190" t="n">
-        <v>21.83</v>
-      </c>
-      <c r="D190" t="n">
-        <v>25.6</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" s="1" t="n">
-        <v>189</v>
-      </c>
-      <c r="B191" t="n">
-        <v>22.67</v>
-      </c>
-      <c r="C191" t="n">
-        <v>21.67</v>
-      </c>
-      <c r="D191" t="n">
-        <v>25.66</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" s="1" t="n">
-        <v>190</v>
-      </c>
-      <c r="B192" t="n">
-        <v>22.75</v>
-      </c>
-      <c r="C192" t="n">
-        <v>21.56</v>
-      </c>
-      <c r="D192" t="n">
-        <v>25.69</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" s="1" t="n">
-        <v>191</v>
-      </c>
-      <c r="B193" t="n">
-        <v>22.83</v>
-      </c>
-      <c r="C193" t="n">
-        <v>21.43</v>
-      </c>
-      <c r="D193" t="n">
-        <v>25.74</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" s="1" t="n">
-        <v>192</v>
-      </c>
-      <c r="B194" t="n">
-        <v>22.92</v>
-      </c>
-      <c r="C194" t="n">
-        <v>21.29</v>
-      </c>
-      <c r="D194" t="n">
-        <v>25.79</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" s="1" t="n">
-        <v>193</v>
-      </c>
-      <c r="B195" t="n">
-        <v>22.92</v>
-      </c>
-      <c r="C195" t="n">
-        <v>21.04</v>
-      </c>
-      <c r="D195" t="n">
-        <v>25.86</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" s="1" t="n">
-        <v>194</v>
-      </c>
-      <c r="B196" t="n">
-        <v>22.86</v>
-      </c>
-      <c r="C196" t="n">
-        <v>20.85</v>
-      </c>
-      <c r="D196" t="n">
-        <v>25.95</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" s="1" t="n">
-        <v>195</v>
-      </c>
-      <c r="B197" t="n">
-        <v>22.71</v>
-      </c>
-      <c r="C197" t="n">
-        <v>20.66</v>
-      </c>
-      <c r="D197" t="n">
-        <v>26.12</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" s="1" t="n">
-        <v>196</v>
-      </c>
-      <c r="B198" t="n">
-        <v>22.6</v>
-      </c>
-      <c r="C198" t="n">
-        <v>20.44</v>
-      </c>
-      <c r="D198" t="n">
-        <v>26.28</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" s="1" t="n">
-        <v>197</v>
-      </c>
-      <c r="B199" t="n">
-        <v>22.52</v>
-      </c>
-      <c r="C199" t="n">
-        <v>20.16</v>
-      </c>
-      <c r="D199" t="n">
-        <v>26.63</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" s="1" t="n">
-        <v>198</v>
-      </c>
-      <c r="B200" t="n">
-        <v>22.46</v>
-      </c>
-      <c r="C200" t="n">
-        <v>19.93</v>
-      </c>
-      <c r="D200" t="n">
-        <v>26.93</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" s="1" t="n">
-        <v>199</v>
-      </c>
-      <c r="B201" t="n">
-        <v>22.54</v>
-      </c>
-      <c r="C201" t="n">
-        <v>19.93</v>
-      </c>
-      <c r="D201" t="n">
-        <v>26.85</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="B202" t="n">
-        <v>22.63</v>
-      </c>
-      <c r="C202" t="n">
-        <v>19.99</v>
-      </c>
-      <c r="D202" t="n">
-        <v>26.7</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="B203" t="n">
-        <v>22.7</v>
-      </c>
-      <c r="C203" t="n">
-        <v>20.06</v>
-      </c>
-      <c r="D203" t="n">
-        <v>26.56</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" s="1" t="n">
-        <v>202</v>
-      </c>
-      <c r="B204" t="n">
-        <v>22.56</v>
-      </c>
-      <c r="C204" t="n">
-        <v>20.12</v>
-      </c>
-      <c r="D204" t="n">
-        <v>26.64</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" s="1" t="n">
-        <v>203</v>
-      </c>
-      <c r="B205" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="C205" t="n">
-        <v>20.28</v>
-      </c>
-      <c r="D205" t="n">
-        <v>26.71</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" s="1" t="n">
-        <v>204</v>
-      </c>
-      <c r="B206" t="n">
-        <v>22.49</v>
-      </c>
-      <c r="C206" t="n">
-        <v>20.39</v>
-      </c>
-      <c r="D206" t="n">
-        <v>26.78</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" s="1" t="n">
-        <v>205</v>
-      </c>
-      <c r="B207" t="n">
-        <v>23.01</v>
-      </c>
-      <c r="C207" t="n">
-        <v>20.11</v>
-      </c>
-      <c r="D207" t="n">
-        <v>26.71</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" s="1" t="n">
-        <v>206</v>
-      </c>
-      <c r="B208" t="n">
-        <v>23.46</v>
-      </c>
-      <c r="C208" t="n">
-        <v>19.89</v>
-      </c>
-      <c r="D208" t="n">
-        <v>26.65</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" s="1" t="n">
-        <v>207</v>
-      </c>
-      <c r="B209" t="n">
-        <v>23.79</v>
-      </c>
-      <c r="C209" t="n">
-        <v>19.67</v>
-      </c>
-      <c r="D209" t="n">
-        <v>26.54</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" s="1" t="n">
-        <v>208</v>
-      </c>
-      <c r="B210" t="n">
-        <v>24.09</v>
-      </c>
-      <c r="C210" t="n">
-        <v>19.37</v>
-      </c>
-      <c r="D210" t="n">
-        <v>26.54</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" s="1" t="n">
-        <v>209</v>
-      </c>
-      <c r="B211" t="n">
-        <v>24.24</v>
-      </c>
-      <c r="C211" t="n">
-        <v>19.13</v>
-      </c>
-      <c r="D211" t="n">
-        <v>26.63</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B212" t="n">
-        <v>24.4</v>
-      </c>
-      <c r="C212" t="n">
-        <v>18.78</v>
-      </c>
-      <c r="D212" t="n">
-        <v>26.81</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="B213" t="n">
-        <v>24.51</v>
-      </c>
-      <c r="C213" t="n">
-        <v>18.58</v>
-      </c>
-      <c r="D213" t="n">
-        <v>26.92</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="B214" t="n">
-        <v>24.76</v>
-      </c>
-      <c r="C214" t="n">
-        <v>18.42</v>
-      </c>
-      <c r="D214" t="n">
-        <v>26.83</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" s="1" t="n">
-        <v>213</v>
-      </c>
-      <c r="B215" t="n">
-        <v>25.02</v>
-      </c>
-      <c r="C215" t="n">
-        <v>18.22</v>
-      </c>
-      <c r="D215" t="n">
-        <v>26.76</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" s="1" t="n">
-        <v>214</v>
-      </c>
-      <c r="B216" t="n">
-        <v>25.34</v>
-      </c>
-      <c r="C216" t="n">
-        <v>18.03</v>
-      </c>
-      <c r="D216" t="n">
-        <v>26.63</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" s="1" t="n">
-        <v>215</v>
-      </c>
-      <c r="B217" t="n">
-        <v>25.25</v>
-      </c>
-      <c r="C217" t="n">
-        <v>18.17</v>
-      </c>
-      <c r="D217" t="n">
-        <v>26.58</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" s="1" t="n">
-        <v>216</v>
-      </c>
-      <c r="B218" t="n">
-        <v>25.79</v>
-      </c>
-      <c r="C218" t="n">
-        <v>18.3</v>
-      </c>
-      <c r="D218" t="n">
-        <v>25.91</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" s="1" t="n">
-        <v>217</v>
-      </c>
-      <c r="B219" t="n">
-        <v>26.56</v>
-      </c>
-      <c r="C219" t="n">
-        <v>18.43</v>
-      </c>
-      <c r="D219" t="n">
-        <v>25.01</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" s="1" t="n">
-        <v>218</v>
-      </c>
-      <c r="B220" t="n">
-        <v>27.51</v>
-      </c>
-      <c r="C220" t="n">
-        <v>18.56</v>
-      </c>
-      <c r="D220" t="n">
-        <v>23.93</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" s="1" t="n">
-        <v>219</v>
-      </c>
-      <c r="B221" t="n">
-        <v>28.46</v>
-      </c>
-      <c r="C221" t="n">
-        <v>18.65</v>
-      </c>
-      <c r="D221" t="n">
-        <v>22.89</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" s="1" t="n">
-        <v>220</v>
-      </c>
-      <c r="B222" t="n">
-        <v>29.35</v>
-      </c>
-      <c r="C222" t="n">
-        <v>18.87</v>
-      </c>
-      <c r="D222" t="n">
-        <v>21.78</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" s="1" t="n">
-        <v>221</v>
-      </c>
-      <c r="B223" t="n">
-        <v>30.29</v>
-      </c>
-      <c r="C223" t="n">
-        <v>18.99</v>
-      </c>
-      <c r="D223" t="n">
-        <v>20.71</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" s="1" t="n">
-        <v>222</v>
-      </c>
-      <c r="B224" t="n">
-        <v>31.29</v>
-      </c>
-      <c r="C224" t="n">
-        <v>19.09</v>
-      </c>
-      <c r="D224" t="n">
-        <v>19.62</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" s="1" t="n">
-        <v>223</v>
-      </c>
-      <c r="B225" t="n">
-        <v>32.21</v>
-      </c>
-      <c r="C225" t="n">
-        <v>18.91</v>
-      </c>
-      <c r="D225" t="n">
-        <v>18.88</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" s="1" t="n">
-        <v>224</v>
-      </c>
-      <c r="B226" t="n">
-        <v>33.02</v>
-      </c>
-      <c r="C226" t="n">
-        <v>17.89</v>
-      </c>
-      <c r="D226" t="n">
-        <v>19.09</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" s="1" t="n">
-        <v>225</v>
-      </c>
-      <c r="B227" t="n">
-        <v>33.57</v>
-      </c>
-      <c r="C227" t="n">
-        <v>16.93</v>
-      </c>
-      <c r="D227" t="n">
-        <v>19.5</v>
+        <v>3.24</v>
+      </c>
+      <c r="E189" t="n">
+        <v>26.07</v>
+      </c>
+      <c r="F189" t="n">
+        <v>9.860000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Progress towards average stats
In progress. Correcting averaging as it seems but not entering dates correctly. Will solve soon
</commit_message>
<xml_diff>
--- a/Outputs/stacks_over_time_avg.xlsx
+++ b/Outputs/stacks_over_time_avg.xlsx
@@ -306,12 +306,12 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>9</col>
+      <col>0</col>
       <colOff>0</colOff>
-      <row>1</row>
+      <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5400000" cy="2700000"/>
+    <ext cx="11520000" cy="6480000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>

</xml_diff>

<commit_message>
Raw and avg nets now available
Program now creates a dataframe containing the net gain/loss of all players during the current session. This data is also sent to Excel and made into a line chart
</commit_message>
<xml_diff>
--- a/Outputs/stacks_over_time_avg.xlsx
+++ b/Outputs/stacks_over_time_avg.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId1"/>
@@ -26,7 +25,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +50,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +75,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -661,7 +674,7 @@
   </sheetPr>
   <dimension ref="A1:F188"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4440,7 +4453,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>